<commit_message>
excell aangevuld + images bijgevoegd
</commit_message>
<xml_diff>
--- a/excel/producten.xlsx
+++ b/excel/producten.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="13340" windowWidth="29440" windowHeight="13400" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="11540" windowWidth="49240" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="221">
   <si>
     <t>id</t>
   </si>
@@ -421,6 +421,282 @@
   </si>
   <si>
     <t>LEATHERMAN_SIGNAL_2C41D52001_7015.jpg</t>
+  </si>
+  <si>
+    <t>SPRAYWAY_CARINA_3124D52019_3030.jpg</t>
+  </si>
+  <si>
+    <t>#BB1933</t>
+  </si>
+  <si>
+    <t>Carina</t>
+  </si>
+  <si>
+    <t>Sprayway</t>
+  </si>
+  <si>
+    <t>#B8152E #287D9D</t>
+  </si>
+  <si>
+    <t>Sapphira</t>
+  </si>
+  <si>
+    <t>SPRAYWAY_SAPPHIRA_3151D42033_4747.jpg</t>
+  </si>
+  <si>
+    <t>#1B6890</t>
+  </si>
+  <si>
+    <t>Limford</t>
+  </si>
+  <si>
+    <t>Vaude</t>
+  </si>
+  <si>
+    <t>3-in-1 Jas</t>
+  </si>
+  <si>
+    <t>#535D75</t>
+  </si>
+  <si>
+    <t>VAUDE_LIMFORD_3353D32003_4141.jpg</t>
+  </si>
+  <si>
+    <t>Lundhags</t>
+  </si>
+  <si>
+    <t>Froso</t>
+  </si>
+  <si>
+    <t>#795F55 #7F7A76</t>
+  </si>
+  <si>
+    <t>Nordald Island</t>
+  </si>
+  <si>
+    <t>Millet</t>
+  </si>
+  <si>
+    <t>MILLET_NORDALD-ISLAND_3351D22017_5656.jpg</t>
+  </si>
+  <si>
+    <t>#A4A191 #6F6F71</t>
+  </si>
+  <si>
+    <t>LUNDHAGS_FROSO_3325D52006_5454.jpg</t>
+  </si>
+  <si>
+    <t>Heritage</t>
+  </si>
+  <si>
+    <t>SPRAYWAY_HERITAGE_3324D42017_4141.jpg</t>
+  </si>
+  <si>
+    <t>#226388 #959698</t>
+  </si>
+  <si>
+    <t>Garmin</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Etrex Touch 25</t>
+  </si>
+  <si>
+    <t>GARMIN_eTrexTouch25_HR_2512C52007.jpg</t>
+  </si>
+  <si>
+    <t>Met gratis batterij t.w.v. € 26,99</t>
+  </si>
+  <si>
+    <t>Wave Limited</t>
+  </si>
+  <si>
+    <t>LEATHERMAN_WAVE_2841d40002_6464_01_be.jpg</t>
+  </si>
+  <si>
+    <t>Bronia</t>
+  </si>
+  <si>
+    <t>100 Glacier</t>
+  </si>
+  <si>
+    <t>THE-NORTH-FACE_GLACIER_3142d30017_7171_10-2.jpg</t>
+  </si>
+  <si>
+    <t>#524B48 #93919E</t>
+  </si>
+  <si>
+    <t>Chimborazo Pro FZ</t>
+  </si>
+  <si>
+    <t>#696B77</t>
+  </si>
+  <si>
+    <t>THE-NORTH-FACE_CHIMBORAZO-PRO_3342d40019_7272_03-2.jpg</t>
+  </si>
+  <si>
+    <t>Jack Wolfskin</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_MADISON_3153D52011_4141.jpg</t>
+  </si>
+  <si>
+    <t>#47546E</t>
+  </si>
+  <si>
+    <t>Peridot</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_PERIDOT_3124D52010_3232.jpg</t>
+  </si>
+  <si>
+    <t>#BD283F #A0A8AB</t>
+  </si>
+  <si>
+    <t>Caribou</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_CARIBOU_3324D52018_4141.jpg</t>
+  </si>
+  <si>
+    <t>#3C84A #999EA2</t>
+  </si>
+  <si>
+    <t>#716A6F</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_MADISON_3353D52013_7171.jpg</t>
+  </si>
+  <si>
+    <t>Crush'n ice</t>
+  </si>
+  <si>
+    <t>Stenton</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_STENTON_3351D52014_7070.jpg</t>
+  </si>
+  <si>
+    <t>#525254</t>
+  </si>
+  <si>
+    <t>Schoudertas</t>
+  </si>
+  <si>
+    <t>Uptown</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_UPTOWN_2311C52002_6767.jpg</t>
+  </si>
+  <si>
+    <t>#44352F</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
+  </si>
+  <si>
+    <t>Heuptas</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_UPGRADE_2361A62004_7070.jpg</t>
+  </si>
+  <si>
+    <t>#3B3B3B</t>
+  </si>
+  <si>
+    <t>Lowa</t>
+  </si>
+  <si>
+    <t>Palermo GTX</t>
+  </si>
+  <si>
+    <t>Winterjas</t>
+  </si>
+  <si>
+    <t>Sarek</t>
+  </si>
+  <si>
+    <t>Frost</t>
+  </si>
+  <si>
+    <t>FJALLRAVEN_SAREK_3153D42049_5454.jpg</t>
+  </si>
+  <si>
+    <t>FJALLRAVEN_FROST_3125D12001_3040.jpg</t>
+  </si>
+  <si>
+    <t>Lada</t>
+  </si>
+  <si>
+    <t>FJALLRAVEN_LADA_3325D22004_7171.jpg</t>
+  </si>
+  <si>
+    <t>#7C7C7A</t>
+  </si>
+  <si>
+    <t>#625249</t>
+  </si>
+  <si>
+    <t>#825166</t>
+  </si>
+  <si>
+    <t>#988E83</t>
+  </si>
+  <si>
+    <t>FJALLRAVEN_LADA_3351d20004_6262_01.jpg</t>
+  </si>
+  <si>
+    <t>Nils</t>
+  </si>
+  <si>
+    <t>Broek</t>
+  </si>
+  <si>
+    <t>FJALLRAVEN_NILS_3381c20001_3030_01.jpg</t>
+  </si>
+  <si>
+    <t>#A56037</t>
+  </si>
+  <si>
+    <t>Rugzak</t>
+  </si>
+  <si>
+    <t>Kanken</t>
+  </si>
+  <si>
+    <t>FJALLRAVEN_KANKEN_2111A80038_4020.jpg</t>
+  </si>
+  <si>
+    <t>#F3BC2C #303B4A #4E524B #7E6246</t>
+  </si>
+  <si>
+    <t>Someone</t>
+  </si>
+  <si>
+    <t>Checkmate</t>
+  </si>
+  <si>
+    <t>SOMEONE_CHECKMATE_4132.jpg</t>
+  </si>
+  <si>
+    <t>ruit_someone.jpg</t>
+  </si>
+  <si>
+    <t>Funny Bunny</t>
+  </si>
+  <si>
+    <t>SOMEONE_FUNNY-BUNNY_1111.jpg</t>
+  </si>
+  <si>
+    <t>#C6B9B #D7ACB #213467 #B8BBC1</t>
   </si>
 </sst>
 </file>
@@ -433,6 +709,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -469,8 +746,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -481,14 +764,20 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -821,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -832,12 +1121,12 @@
     <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
@@ -1687,6 +1976,9 @@
       <c r="N24">
         <v>1</v>
       </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
       <c r="R24">
         <v>1</v>
       </c>
@@ -1713,6 +2005,12 @@
       <c r="H25">
         <v>179.95</v>
       </c>
+      <c r="I25" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
       <c r="R25">
         <v>1</v>
       </c>
@@ -1724,6 +2022,898 @@
       </c>
       <c r="V25" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22">
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G26">
+        <v>69.95</v>
+      </c>
+      <c r="H26">
+        <v>49</v>
+      </c>
+      <c r="I26" t="s">
+        <v>133</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="V26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22">
+      <c r="B27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" t="s">
+        <v>135</v>
+      </c>
+      <c r="G27">
+        <v>149.94999999999999</v>
+      </c>
+      <c r="H27">
+        <v>109</v>
+      </c>
+      <c r="I27" t="s">
+        <v>136</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="V27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22">
+      <c r="B28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G28">
+        <v>199.95</v>
+      </c>
+      <c r="H28">
+        <v>139</v>
+      </c>
+      <c r="I28" t="s">
+        <v>140</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="V28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22">
+      <c r="B29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29">
+        <v>99.95</v>
+      </c>
+      <c r="H29">
+        <v>69</v>
+      </c>
+      <c r="I29" t="s">
+        <v>144</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="V29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22">
+      <c r="B30" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30">
+        <v>279.95</v>
+      </c>
+      <c r="H30">
+        <v>189</v>
+      </c>
+      <c r="I30" t="s">
+        <v>148</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="V30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22">
+      <c r="B31" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" t="s">
+        <v>151</v>
+      </c>
+      <c r="G31">
+        <v>94.95</v>
+      </c>
+      <c r="H31">
+        <v>64</v>
+      </c>
+      <c r="I31" t="s">
+        <v>152</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="V31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22">
+      <c r="B32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" t="s">
+        <v>156</v>
+      </c>
+      <c r="H32">
+        <v>249</v>
+      </c>
+      <c r="J32" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="V32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22">
+      <c r="B33" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" t="s">
+        <v>159</v>
+      </c>
+      <c r="H33">
+        <v>99.95</v>
+      </c>
+      <c r="J33" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="V33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22">
+      <c r="B34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34">
+        <v>99.95</v>
+      </c>
+      <c r="H34">
+        <v>69</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="V34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="2:22">
+      <c r="B35" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35">
+        <v>69.95</v>
+      </c>
+      <c r="H35">
+        <v>49</v>
+      </c>
+      <c r="I35" t="s">
+        <v>163</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="V35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22">
+      <c r="B36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" t="s">
+        <v>166</v>
+      </c>
+      <c r="G36">
+        <v>99.95</v>
+      </c>
+      <c r="H36">
+        <v>69</v>
+      </c>
+      <c r="I36" t="s">
+        <v>165</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="V36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="2:22">
+      <c r="B37" t="s">
+        <v>168</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>167</v>
+      </c>
+      <c r="E37" t="s">
+        <v>169</v>
+      </c>
+      <c r="G37">
+        <v>119.95</v>
+      </c>
+      <c r="H37">
+        <v>69</v>
+      </c>
+      <c r="I37" t="s">
+        <v>170</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+      <c r="V37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="2:22">
+      <c r="B38" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G38">
+        <v>99.95</v>
+      </c>
+      <c r="H38">
+        <v>59</v>
+      </c>
+      <c r="I38" t="s">
+        <v>173</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="V38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22">
+      <c r="B39" t="s">
+        <v>174</v>
+      </c>
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" t="s">
+        <v>175</v>
+      </c>
+      <c r="G39">
+        <v>99.95</v>
+      </c>
+      <c r="H39">
+        <v>59</v>
+      </c>
+      <c r="I39" t="s">
+        <v>176</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="V39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22">
+      <c r="B40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" t="s">
+        <v>178</v>
+      </c>
+      <c r="G40">
+        <v>119.95</v>
+      </c>
+      <c r="H40">
+        <v>69</v>
+      </c>
+      <c r="I40" t="s">
+        <v>177</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="V40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="2:22">
+      <c r="B41" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>167</v>
+      </c>
+      <c r="G41">
+        <v>199.95</v>
+      </c>
+      <c r="H41">
+        <v>124</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="V41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="2:22">
+      <c r="B42" t="s">
+        <v>180</v>
+      </c>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" t="s">
+        <v>167</v>
+      </c>
+      <c r="E42" t="s">
+        <v>181</v>
+      </c>
+      <c r="I42" t="s">
+        <v>182</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+      <c r="V42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22">
+      <c r="B43" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43" t="s">
+        <v>183</v>
+      </c>
+      <c r="D43" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" t="s">
+        <v>185</v>
+      </c>
+      <c r="H43">
+        <v>49.95</v>
+      </c>
+      <c r="I43" t="s">
+        <v>186</v>
+      </c>
+      <c r="J43" t="s">
+        <v>59</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="R43">
+        <v>1</v>
+      </c>
+      <c r="V43" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="2:22">
+      <c r="B44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" t="s">
+        <v>189</v>
+      </c>
+      <c r="D44" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H44">
+        <v>29.95</v>
+      </c>
+      <c r="I44" t="s">
+        <v>191</v>
+      </c>
+      <c r="J44" t="s">
+        <v>48</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="V44" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="2:22">
+      <c r="B45" t="s">
+        <v>193</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" t="s">
+        <v>192</v>
+      </c>
+      <c r="G45">
+        <v>129.94999999999999</v>
+      </c>
+      <c r="H45">
+        <v>99</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+      <c r="V45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22">
+      <c r="B46" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" t="s">
+        <v>192</v>
+      </c>
+      <c r="G46">
+        <v>129.94999999999999</v>
+      </c>
+      <c r="H46">
+        <v>99</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+      <c r="V46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="2:22">
+      <c r="B47" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47" t="s">
+        <v>194</v>
+      </c>
+      <c r="D47" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" t="s">
+        <v>197</v>
+      </c>
+      <c r="H47">
+        <v>399.95</v>
+      </c>
+      <c r="I47" t="s">
+        <v>202</v>
+      </c>
+      <c r="J47" t="s">
+        <v>48</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+      <c r="V47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="2:22">
+      <c r="B48" t="s">
+        <v>196</v>
+      </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" t="s">
+        <v>198</v>
+      </c>
+      <c r="H48">
+        <v>159.94999999999999</v>
+      </c>
+      <c r="I48" t="s">
+        <v>203</v>
+      </c>
+      <c r="J48" t="s">
+        <v>48</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+      <c r="V48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="2:22">
+      <c r="B49" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" t="s">
+        <v>200</v>
+      </c>
+      <c r="H49">
+        <v>149.94999999999999</v>
+      </c>
+      <c r="I49" t="s">
+        <v>201</v>
+      </c>
+      <c r="J49" t="s">
+        <v>48</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+      <c r="V49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="2:22">
+      <c r="B50" t="s">
+        <v>199</v>
+      </c>
+      <c r="C50" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" t="s">
+        <v>205</v>
+      </c>
+      <c r="H50">
+        <v>149.94999999999999</v>
+      </c>
+      <c r="I50" t="s">
+        <v>204</v>
+      </c>
+      <c r="J50" t="s">
+        <v>48</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+      <c r="V50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="2:22">
+      <c r="B51" t="s">
+        <v>206</v>
+      </c>
+      <c r="C51" t="s">
+        <v>207</v>
+      </c>
+      <c r="D51" t="s">
+        <v>76</v>
+      </c>
+      <c r="E51" t="s">
+        <v>208</v>
+      </c>
+      <c r="H51">
+        <v>129.94999999999999</v>
+      </c>
+      <c r="I51" t="s">
+        <v>209</v>
+      </c>
+      <c r="J51" t="s">
+        <v>48</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="Q51">
+        <v>1</v>
+      </c>
+      <c r="V51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="2:22">
+      <c r="B52" t="s">
+        <v>211</v>
+      </c>
+      <c r="C52" t="s">
+        <v>210</v>
+      </c>
+      <c r="D52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" t="s">
+        <v>212</v>
+      </c>
+      <c r="H52">
+        <v>79.95</v>
+      </c>
+      <c r="I52" t="s">
+        <v>213</v>
+      </c>
+      <c r="J52" t="s">
+        <v>48</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="R52">
+        <v>1</v>
+      </c>
+      <c r="V52" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="2:22">
+      <c r="B53" t="s">
+        <v>215</v>
+      </c>
+      <c r="C53" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" t="s">
+        <v>214</v>
+      </c>
+      <c r="E53" t="s">
+        <v>216</v>
+      </c>
+      <c r="G53">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="H53">
+        <v>25</v>
+      </c>
+      <c r="I53" t="s">
+        <v>217</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+      <c r="P53">
+        <v>1</v>
+      </c>
+      <c r="V53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="2:22">
+      <c r="B54" t="s">
+        <v>218</v>
+      </c>
+      <c r="C54" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" t="s">
+        <v>214</v>
+      </c>
+      <c r="E54" t="s">
+        <v>219</v>
+      </c>
+      <c r="G54">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="H54">
+        <v>25</v>
+      </c>
+      <c r="I54" t="s">
+        <v>220</v>
+      </c>
+      <c r="O54">
+        <v>1</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="V54" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mising product-images part 1
</commit_message>
<xml_diff>
--- a/excel/producten.xlsx
+++ b/excel/producten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="0" windowWidth="41320" windowHeight="26360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19600" windowHeight="25260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="producten.csv" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="304">
   <si>
     <t>id</t>
   </si>
@@ -931,6 +931,33 @@
   </si>
   <si>
     <t>2541d52001_6210_01_be.jpg</t>
+  </si>
+  <si>
+    <t>VAUDE_BRONIA_3124D52007_7272.jpg</t>
+  </si>
+  <si>
+    <t>RAYBAN_ZONNEBRIL_2212a80015_6262_01.jpg</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_MADISON_3153D52011_4141.jpg</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_MADISON_3353D52013_7171.jpg</t>
+  </si>
+  <si>
+    <t>JACK-WOLFSKIN_CRUSH-'N-ICE_31B1D30005_4848.jpg</t>
+  </si>
+  <si>
+    <t>LOWA_PALERMO-MEN_3722D52001_6060_01.jpg</t>
+  </si>
+  <si>
+    <t>LOWA_PALERMO-WOMEN_3712D52001_6090_01.jpg</t>
+  </si>
+  <si>
+    <t>STONESBONES_LAMA_5311D52122_5526.jpg</t>
+  </si>
+  <si>
+    <t>CANNONDALE_TESORO-2_A213C52007_4141-2.jpg</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1393,7 @@
       <pane xSplit="8" ySplit="37" topLeftCell="I38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1386,7 +1413,7 @@
     <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -1537,10 +1564,11 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <f>P2+3</f>
+        <v>4</v>
       </c>
       <c r="U3" t="s">
         <v>15</v>
@@ -1578,10 +1606,10 @@
         <v>1</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U4" t="s">
         <v>15</v>
@@ -1619,10 +1647,10 @@
         <v>1</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U5" t="s">
         <v>15</v>
@@ -1660,10 +1688,11 @@
         <v>1</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <f>P5+3</f>
+        <v>13</v>
       </c>
       <c r="U6" t="s">
         <v>15</v>
@@ -1698,13 +1727,13 @@
         <v>45</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="N7">
         <v>1</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="T7">
         <v>1</v>
@@ -1742,10 +1771,10 @@
         <v>45</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="T8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U8" t="s">
         <v>15</v>
@@ -1780,10 +1809,10 @@
         <v>55</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="U9" t="s">
         <v>15</v>
@@ -1815,10 +1844,10 @@
         <v>60</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="U10" t="s">
         <v>15</v>
@@ -1853,10 +1882,10 @@
         <v>64</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="P11">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="U11" t="s">
         <v>15</v>
@@ -1894,10 +1923,10 @@
         <v>1</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="U12" t="s">
         <v>15</v>
@@ -1929,10 +1958,10 @@
         <v>72</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -1967,13 +1996,13 @@
         <v>76</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="P14">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U14" t="s">
         <v>15</v>
@@ -1992,6 +2021,9 @@
       <c r="D15" t="s">
         <v>78</v>
       </c>
+      <c r="E15" t="s">
+        <v>296</v>
+      </c>
       <c r="H15">
         <v>124.95</v>
       </c>
@@ -1999,16 +2031,16 @@
         <v>79</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U15" t="s">
         <v>15</v>
@@ -2043,10 +2075,10 @@
         <v>84</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -2084,10 +2116,10 @@
         <v>91</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U17" t="s">
         <v>88</v>
@@ -2122,10 +2154,10 @@
         <v>92</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U18" t="s">
         <v>88</v>
@@ -2160,10 +2192,10 @@
         <v>45</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="Q19">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="U19" t="s">
         <v>88</v>
@@ -2195,13 +2227,13 @@
         <v>45</v>
       </c>
       <c r="N20">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="P20">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="U20" t="s">
         <v>88</v>
@@ -2236,10 +2268,10 @@
         <v>101</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="Q21">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="U21" t="s">
         <v>88</v>
@@ -2274,13 +2306,13 @@
         <v>106</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="N22">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="R22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U22" t="s">
         <v>88</v>
@@ -2315,13 +2347,13 @@
         <v>45</v>
       </c>
       <c r="M23">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="P23">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="Q23">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="U23" t="s">
         <v>88</v>
@@ -2356,13 +2388,13 @@
         <v>113</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="R24">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U24" t="s">
         <v>88</v>
@@ -2394,10 +2426,10 @@
         <v>119</v>
       </c>
       <c r="R25">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="T25">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="U25" t="s">
         <v>88</v>
@@ -2432,10 +2464,10 @@
         <v>122</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="Q26">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="U26" t="s">
         <v>88</v>
@@ -2470,10 +2502,10 @@
         <v>125</v>
       </c>
       <c r="M27">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="Q27">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="U27" t="s">
         <v>88</v>
@@ -2508,10 +2540,10 @@
         <v>128</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="Q28">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="U28" t="s">
         <v>88</v>
@@ -2546,10 +2578,10 @@
         <v>132</v>
       </c>
       <c r="N29">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="Q29">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="U29" t="s">
         <v>88</v>
@@ -2584,10 +2616,10 @@
         <v>136</v>
       </c>
       <c r="N30">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="Q30">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="U30" t="s">
         <v>88</v>
@@ -2622,10 +2654,10 @@
         <v>140</v>
       </c>
       <c r="N31">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="Q31">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="U31" t="s">
         <v>88</v>
@@ -2657,10 +2689,10 @@
         <v>145</v>
       </c>
       <c r="R32">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="T32">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="U32" t="s">
         <v>88</v>
@@ -2698,10 +2730,10 @@
         <v>1</v>
       </c>
       <c r="R33">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="T33">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="U33" t="s">
         <v>88</v>
@@ -2723,6 +2755,9 @@
       <c r="D34" t="s">
         <v>127</v>
       </c>
+      <c r="E34" t="s">
+        <v>295</v>
+      </c>
       <c r="G34">
         <v>99.95</v>
       </c>
@@ -2730,10 +2765,10 @@
         <v>69</v>
       </c>
       <c r="M34">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="Q34">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="U34" t="s">
         <v>88</v>
@@ -2768,10 +2803,10 @@
         <v>151</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="Q35">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="U35" t="s">
         <v>88</v>
@@ -2806,10 +2841,10 @@
         <v>153</v>
       </c>
       <c r="N36">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="Q36">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="U36" t="s">
         <v>88</v>
@@ -2831,6 +2866,9 @@
       <c r="D37" t="s">
         <v>155</v>
       </c>
+      <c r="E37" t="s">
+        <v>297</v>
+      </c>
       <c r="G37">
         <v>119.95</v>
       </c>
@@ -2838,10 +2876,10 @@
         <v>69</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>142</v>
       </c>
       <c r="Q37">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="U37" t="s">
         <v>88</v>
@@ -2863,6 +2901,9 @@
       <c r="D38" t="s">
         <v>155</v>
       </c>
+      <c r="E38" t="s">
+        <v>298</v>
+      </c>
       <c r="G38">
         <v>119.95</v>
       </c>
@@ -2870,10 +2911,10 @@
         <v>69</v>
       </c>
       <c r="N38">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="Q38">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="U38" t="s">
         <v>88</v>
@@ -2908,10 +2949,10 @@
         <v>159</v>
       </c>
       <c r="M39">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="Q39">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="U39" t="s">
         <v>88</v>
@@ -2946,10 +2987,10 @@
         <v>162</v>
       </c>
       <c r="M40">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="Q40">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="U40" t="s">
         <v>88</v>
@@ -2971,6 +3012,9 @@
       <c r="D41" t="s">
         <v>155</v>
       </c>
+      <c r="E41" t="s">
+        <v>299</v>
+      </c>
       <c r="G41">
         <v>199.95</v>
       </c>
@@ -2978,10 +3022,10 @@
         <v>124</v>
       </c>
       <c r="M41">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="Q41">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="U41" t="s">
         <v>88</v>
@@ -3010,10 +3054,10 @@
         <v>166</v>
       </c>
       <c r="N42">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="Q42">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="U42" t="s">
         <v>88</v>
@@ -3048,10 +3092,10 @@
         <v>55</v>
       </c>
       <c r="M43">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="R43">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="U43" t="s">
         <v>88</v>
@@ -3086,13 +3130,13 @@
         <v>45</v>
       </c>
       <c r="M44">
-        <v>1</v>
+        <v>157</v>
       </c>
       <c r="N44">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="R44">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="U44" t="s">
         <v>88</v>
@@ -3114,6 +3158,9 @@
       <c r="D45" t="s">
         <v>175</v>
       </c>
+      <c r="E45" t="s">
+        <v>300</v>
+      </c>
       <c r="G45">
         <v>129.94999999999999</v>
       </c>
@@ -3121,10 +3168,10 @@
         <v>99</v>
       </c>
       <c r="M45">
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="Q45">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="U45" t="s">
         <v>88</v>
@@ -3146,6 +3193,9 @@
       <c r="D46" t="s">
         <v>175</v>
       </c>
+      <c r="E46" t="s">
+        <v>301</v>
+      </c>
       <c r="G46">
         <v>129.94999999999999</v>
       </c>
@@ -3153,10 +3203,10 @@
         <v>99</v>
       </c>
       <c r="N46">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="Q46">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="U46" t="s">
         <v>88</v>
@@ -3191,10 +3241,10 @@
         <v>45</v>
       </c>
       <c r="M47">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="Q47">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="U47" t="s">
         <v>88</v>
@@ -3229,10 +3279,10 @@
         <v>45</v>
       </c>
       <c r="M48">
-        <v>1</v>
+        <v>166</v>
       </c>
       <c r="Q48">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="U48" t="s">
         <v>88</v>
@@ -3267,10 +3317,10 @@
         <v>45</v>
       </c>
       <c r="N49">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="Q49">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="U49" t="s">
         <v>88</v>
@@ -3305,10 +3355,10 @@
         <v>45</v>
       </c>
       <c r="N50">
-        <v>1</v>
+        <v>149</v>
       </c>
       <c r="Q50">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="U50" t="s">
         <v>88</v>
@@ -3343,16 +3393,16 @@
         <v>79</v>
       </c>
       <c r="M51">
-        <v>1</v>
+        <v>168</v>
       </c>
       <c r="N51">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="P51">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="R51">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="U51" t="s">
         <v>88</v>
@@ -3393,7 +3443,7 @@
         <v>1</v>
       </c>
       <c r="P52">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="U52" t="s">
         <v>281</v>
@@ -3428,7 +3478,7 @@
         <v>1</v>
       </c>
       <c r="P53">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="U53" t="s">
         <v>281</v>
@@ -3466,7 +3516,7 @@
         <v>1</v>
       </c>
       <c r="P54">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="U54" t="s">
         <v>281</v>
@@ -3507,7 +3557,7 @@
         <v>1</v>
       </c>
       <c r="P55">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="U55" t="s">
         <v>281</v>
@@ -3529,6 +3579,9 @@
       <c r="D56" t="s">
         <v>206</v>
       </c>
+      <c r="E56" t="s">
+        <v>302</v>
+      </c>
       <c r="G56">
         <v>24.95</v>
       </c>
@@ -3542,7 +3595,7 @@
         <v>1</v>
       </c>
       <c r="P56">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="U56" t="s">
         <v>281</v>
@@ -3583,7 +3636,7 @@
         <v>1</v>
       </c>
       <c r="P57">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="U57" t="s">
         <v>281</v>
@@ -3621,10 +3674,10 @@
         <v>1</v>
       </c>
       <c r="P58">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="Q58">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="U58" t="s">
         <v>281</v>
@@ -3662,7 +3715,7 @@
         <v>1</v>
       </c>
       <c r="R59">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="U59" t="s">
         <v>281</v>
@@ -3684,6 +3737,9 @@
       <c r="D60" t="s">
         <v>141</v>
       </c>
+      <c r="E60" t="s">
+        <v>144</v>
+      </c>
       <c r="H60">
         <v>169</v>
       </c>
@@ -3691,13 +3747,13 @@
         <v>45</v>
       </c>
       <c r="R60">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="S60">
         <v>1</v>
       </c>
       <c r="T60">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="U60" t="s">
         <v>216</v>
@@ -3719,6 +3775,9 @@
       <c r="D61" t="s">
         <v>218</v>
       </c>
+      <c r="E61" t="s">
+        <v>303</v>
+      </c>
       <c r="H61" s="1">
         <v>1299</v>
       </c>
@@ -3726,10 +3785,13 @@
         <v>289</v>
       </c>
       <c r="N61">
-        <v>1</v>
+        <v>201</v>
+      </c>
+      <c r="R61">
+        <v>33</v>
       </c>
       <c r="S61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U61" t="s">
         <v>216</v>
@@ -3758,13 +3820,13 @@
         <v>45</v>
       </c>
       <c r="R62">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="S62">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T62">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="U62" t="s">
         <v>216</v>
@@ -3799,7 +3861,7 @@
         <v>230</v>
       </c>
       <c r="S63">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U63" t="s">
         <v>216</v>
@@ -3834,10 +3896,10 @@
         <v>229</v>
       </c>
       <c r="N64">
-        <v>1</v>
+        <v>205</v>
       </c>
       <c r="S64">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="U64" t="s">
         <v>216</v>
@@ -3866,10 +3928,10 @@
         <v>99</v>
       </c>
       <c r="N65">
-        <v>1</v>
+        <v>207</v>
       </c>
       <c r="S65">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="U65" t="s">
         <v>216</v>
@@ -3898,13 +3960,13 @@
         <v>45</v>
       </c>
       <c r="M66">
-        <v>1</v>
+        <v>172</v>
       </c>
       <c r="N66">
-        <v>1</v>
+        <v>210</v>
       </c>
       <c r="S66">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="U66" t="s">
         <v>216</v>
@@ -3933,10 +3995,10 @@
         <v>237</v>
       </c>
       <c r="N67">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="T67">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="U67" t="s">
         <v>18</v>
@@ -3962,10 +4024,10 @@
         <v>29.95</v>
       </c>
       <c r="N68">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="T68">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="U68" t="s">
         <v>18</v>
@@ -3988,10 +4050,10 @@
         <v>19.95</v>
       </c>
       <c r="N69">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="T69">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="U69" t="s">
         <v>18</v>
@@ -4014,10 +4076,10 @@
         <v>24.95</v>
       </c>
       <c r="N70">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="T70">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="U70" t="s">
         <v>18</v>
@@ -4040,10 +4102,10 @@
         <v>24.95</v>
       </c>
       <c r="N71">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="T71">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="U71" t="s">
         <v>18</v>
@@ -4066,10 +4128,10 @@
         <v>24.95</v>
       </c>
       <c r="N72">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="T72">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="U72" t="s">
         <v>18</v>
@@ -4092,10 +4154,10 @@
         <v>19.95</v>
       </c>
       <c r="N73">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="T73">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="U73" t="s">
         <v>18</v>
@@ -4118,10 +4180,10 @@
         <v>29.95</v>
       </c>
       <c r="N74">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="T74">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="U74" t="s">
         <v>18</v>
@@ -4144,10 +4206,10 @@
         <v>24.95</v>
       </c>
       <c r="N75">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="T75">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="U75" t="s">
         <v>18</v>
@@ -4172,14 +4234,11 @@
       <c r="H76">
         <v>449</v>
       </c>
-      <c r="N76">
-        <v>1</v>
-      </c>
       <c r="R76">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="T76">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="U76" t="s">
         <v>18</v>
@@ -4202,10 +4261,10 @@
         <v>19.95</v>
       </c>
       <c r="N77">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="T77">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="U77" t="s">
         <v>18</v>
@@ -4228,10 +4287,10 @@
         <v>19.95</v>
       </c>
       <c r="N78">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="T78">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="U78" t="s">
         <v>18</v>
@@ -4260,7 +4319,7 @@
         <v>55</v>
       </c>
       <c r="T79">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="U79" t="s">
         <v>18</v>
@@ -4283,10 +4342,10 @@
         <v>256</v>
       </c>
       <c r="R80">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="T80">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="U80" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
links en productimages toegevoegd
</commit_message>
<xml_diff>
--- a/excel/producten.xlsx
+++ b/excel/producten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19600" windowHeight="25260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40980" windowHeight="25260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="producten.csv" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="366">
   <si>
     <t>id</t>
   </si>
@@ -959,12 +959,222 @@
   <si>
     <t>CANNONDALE_TESORO-2_A213C52007_4141-2.jpg</t>
   </si>
+  <si>
+    <t>/jack-wolfskin-schoudertas-uptown-2311c52002?id_colour=4090</t>
+  </si>
+  <si>
+    <t>/jack-wolfskin-heuptas-upgrade-2361a62004?id_colour=4168</t>
+  </si>
+  <si>
+    <t>/lowa-schoen-palermo-gore-tex-3722d52001?id_colour=3544</t>
+  </si>
+  <si>
+    <r>
+      <t>/fjaellraeven-jas-sarek-winter-3153d42049</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?id_colour=3856</t>
+    </r>
+  </si>
+  <si>
+    <t>/fjaellraeven-trui-frost-dames-3125d12001?id_colour=1448</t>
+  </si>
+  <si>
+    <t>/fjaellraeven-trui-lada-3325d22004?id_colour=4246</t>
+  </si>
+  <si>
+    <t>/fjaellraeven-broek-nils-3341c22001?id_colour=1438</t>
+  </si>
+  <si>
+    <r>
+      <t>/fjaellraeven-dagrugzak-kanken-2111a80038</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?id_colour=1594</t>
+    </r>
+  </si>
+  <si>
+    <t>/tumble-n-dry-broek-antonius-sweat-pant-5374d52016?id_colour=4246</t>
+  </si>
+  <si>
+    <t>/stones-bones-t-shirt-mr-lama-5311d52122?id_colour=3360</t>
+  </si>
+  <si>
+    <t>/petit-louie-jurk-nara-cross-5261d52001?id_colour=2805</t>
+  </si>
+  <si>
+    <t>/jack-wolfskin-jas-zenon-kids-5184d42001?id_colour=1988</t>
+  </si>
+  <si>
+    <t>/jack-wolfskin-dagrugzak-little-joe-2121c22002?id_colour=1474</t>
+  </si>
+  <si>
+    <t>/garmin-gps-etrex-touch-25-2512c52007?id_colour=2397</t>
+  </si>
+  <si>
+    <t>/cannondale-citybike-tesoro-2-a213c52007?id_colour=2296</t>
+  </si>
+  <si>
+    <t>/ortlieb-fietstas-achter-back-roller-urban-a513c52002?id_colour=2608</t>
+  </si>
+  <si>
+    <t>/rh-windstopper-blowy-9221d42011?id_colour=4168</t>
+  </si>
+  <si>
+    <t>/gore-bike-wear-softshell-contest-so-9222b92003?id_colour=780</t>
+  </si>
+  <si>
+    <t>/vaude-broek-fluid-ii-9235b82003?id_colour=4168</t>
+  </si>
+  <si>
+    <t>/garmin-gps-fenix-3-2512c52003?id_colour=4324</t>
+  </si>
+  <si>
+    <t>/xtorm-oplader-waterproof-xtreme-9000-2g31d42013?id_colour=5806</t>
+  </si>
+  <si>
+    <t>/yaya-jumpsuit-021634-4198d52016?id_colour=4118</t>
+  </si>
+  <si>
+    <t>/king-louie-jurk-balance-cross-4162d52032?id_colour=2117</t>
+  </si>
+  <si>
+    <t>/king-louie-jurk-nara-cross-4162d52033?id_colour=2548</t>
+  </si>
+  <si>
+    <t>/king-louie-cardigan-flower-lurex-4144d52101?id_colour=2530</t>
+  </si>
+  <si>
+    <t>/wewood-horloge-date-2541d52001?id_colour=3656</t>
+  </si>
+  <si>
+    <t>/kikkerland-gadget-bird-is-the-word-jewelry-holder-2h41c52043?id_colour=4168</t>
+  </si>
+  <si>
+    <t>/premium-jas-timmy-4355d52026?id_colour=2140</t>
+  </si>
+  <si>
+    <t>/blend-trui-20700314-4349d52042?id_colour=2270</t>
+  </si>
+  <si>
+    <t>/ichi-jas-tri-4153d52055?id_colour=2306</t>
+  </si>
+  <si>
+    <t>/fjaellraeven-jas-greenland-no-1-down-3352d42051?id_colour=2297</t>
+  </si>
+  <si>
+    <t>/camel-active-bags-portefeuille-165703-2392c52011?id_colour=3622</t>
+  </si>
+  <si>
+    <t>/ayacucho-jas-highland-padded-3353d52016?id_colour=2764</t>
+  </si>
+  <si>
+    <t>/ayacucho-fleece-inverno-280-3124d42016?id_colour=2920</t>
+  </si>
+  <si>
+    <t>/osprey-reistas-porter-46-2221d42002?id_colour=4169</t>
+  </si>
+  <si>
+    <t>/ayacucho-jas-stowaway-3157d52001?id_colour=4422</t>
+  </si>
+  <si>
+    <t>/ayacucho-dagrugzak-mojave-28-ii-1212c10002?id_colour=4168</t>
+  </si>
+  <si>
+    <t>/leatherman-multitool-signal-2c41d52001?id_colour=4123</t>
+  </si>
+  <si>
+    <t>/sprayway-fleece-carina-3124d52019?id_colour=1438</t>
+  </si>
+  <si>
+    <t>/sprayway-jas-sapphira-3-in-1-3151d42033?id_colour=3154</t>
+  </si>
+  <si>
+    <t>/lundhags-trui-froso-3325d52006?id_colour=3310</t>
+  </si>
+  <si>
+    <t>/millet-jas-nordald-island-3-in-1-3351d22017?id_colour=3466</t>
+  </si>
+  <si>
+    <t>/leatherman-multitool-wave-2c41d42001?id_colour=3856</t>
+  </si>
+  <si>
+    <t>/the-north-face-fleece-chimborazo-pro-3324d42009?id_colour=4324</t>
+  </si>
+  <si>
+    <t>GBW_CONTEST-SO_7732B90002_3030.jpg</t>
+  </si>
+  <si>
+    <t>LEZYNE_MACRO-DRIVE-600_A372C52002_7070.jpg</t>
+  </si>
+  <si>
+    <t>VAUDE_FLUID-II_7745b80004_7070_01.jpg</t>
+  </si>
+  <si>
+    <t>Contigo-packshot.jpg</t>
+  </si>
+  <si>
+    <t>IZOLA_ShotGlasses_IMG_1894-2-2.jpg</t>
+  </si>
+  <si>
+    <t>#D82B46 #F2F1F0</t>
+  </si>
+  <si>
+    <t>MENS_SOCIETY_WISKEY_CUBES-2015-120-2.jpg</t>
+  </si>
+  <si>
+    <t>IZOLA_RDAW-140522-Izola-Money-Clip-logo-living-well-1.jpg</t>
+  </si>
+  <si>
+    <t>IZOLA_RDAW-140526-Izola-Shoehorn-Logo-talk-the-talk-1.jpg</t>
+  </si>
+  <si>
+    <t>IZOLA_ShoeBag_DifShoes.jpg</t>
+  </si>
+  <si>
+    <t>MENS_SOCIETY_SHOE-SHINE-KIT-64-2.jpg</t>
+  </si>
+  <si>
+    <t>MENS_SOCIETY_STOW-AWAY-TRAVEL-KIT_-2015-14.jpg</t>
+  </si>
+  <si>
+    <t>MENS_SOCIETY_HANDSOME-HANDS-MANICURE-SET-2015-9.jpg</t>
+  </si>
+  <si>
+    <t>GARMIN_FENIX-3_2452c50001_7272_01.jpg_be.jpg</t>
+  </si>
+  <si>
+    <t>IZOLA_Brusches_BFA_2908.jpg</t>
+  </si>
+  <si>
+    <t>IZOLA_3203_TravelCup_Canoe.jpg</t>
+  </si>
+  <si>
+    <t>XTORM_XTREME-9000_2b31d40016_0101_03_be.jpg</t>
+  </si>
+  <si>
+    <t>TOMTOM_RUNNER2CARDIO+MUSIC_.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -984,6 +1194,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1390,10 +1607,10 @@
   <dimension ref="A1:W80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="37" topLeftCell="I38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="37" topLeftCell="K38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
-      <selection pane="bottomRight" activeCell="E62" sqref="E62"/>
+      <selection pane="bottomRight" activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1403,7 +1620,7 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="54.83203125" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="46.5" customWidth="1"/>
@@ -1551,6 +1768,9 @@
       <c r="E3" t="s">
         <v>28</v>
       </c>
+      <c r="F3" t="s">
+        <v>325</v>
+      </c>
       <c r="G3">
         <v>89.95</v>
       </c>
@@ -1593,6 +1813,9 @@
       <c r="E4" t="s">
         <v>34</v>
       </c>
+      <c r="F4" t="s">
+        <v>326</v>
+      </c>
       <c r="G4">
         <v>79.989999999999995</v>
       </c>
@@ -1634,6 +1857,9 @@
       <c r="E5" t="s">
         <v>36</v>
       </c>
+      <c r="F5" t="s">
+        <v>327</v>
+      </c>
       <c r="G5">
         <v>79.989999999999995</v>
       </c>
@@ -1675,6 +1901,9 @@
       <c r="E6" t="s">
         <v>40</v>
       </c>
+      <c r="F6" t="s">
+        <v>328</v>
+      </c>
       <c r="G6">
         <v>69.989999999999995</v>
       </c>
@@ -1717,6 +1946,9 @@
       <c r="E7" t="s">
         <v>294</v>
       </c>
+      <c r="F7" t="s">
+        <v>329</v>
+      </c>
       <c r="H7">
         <v>99.95</v>
       </c>
@@ -1761,6 +1993,9 @@
       <c r="E8" t="s">
         <v>50</v>
       </c>
+      <c r="F8" t="s">
+        <v>330</v>
+      </c>
       <c r="H8">
         <v>8.9499999999999993</v>
       </c>
@@ -1799,6 +2034,9 @@
       <c r="E9" t="s">
         <v>54</v>
       </c>
+      <c r="F9" t="s">
+        <v>331</v>
+      </c>
       <c r="H9">
         <v>49.99</v>
       </c>
@@ -1872,6 +2110,9 @@
       <c r="E11" t="s">
         <v>63</v>
       </c>
+      <c r="F11" t="s">
+        <v>332</v>
+      </c>
       <c r="G11">
         <v>69.95</v>
       </c>
@@ -1910,6 +2151,9 @@
       <c r="E12" t="s">
         <v>67</v>
       </c>
+      <c r="F12" t="s">
+        <v>333</v>
+      </c>
       <c r="G12">
         <v>149</v>
       </c>
@@ -1951,6 +2195,9 @@
       <c r="E13" t="s">
         <v>71</v>
       </c>
+      <c r="F13" t="s">
+        <v>334</v>
+      </c>
       <c r="H13">
         <v>499.95</v>
       </c>
@@ -1986,6 +2233,9 @@
       <c r="E14" t="s">
         <v>75</v>
       </c>
+      <c r="F14" t="s">
+        <v>335</v>
+      </c>
       <c r="G14">
         <v>49.95</v>
       </c>
@@ -2182,6 +2432,9 @@
       <c r="E19" t="s">
         <v>95</v>
       </c>
+      <c r="F19" t="s">
+        <v>336</v>
+      </c>
       <c r="H19">
         <v>169.95</v>
       </c>
@@ -2258,6 +2511,9 @@
       <c r="E21" t="s">
         <v>100</v>
       </c>
+      <c r="F21" t="s">
+        <v>337</v>
+      </c>
       <c r="G21">
         <v>59.95</v>
       </c>
@@ -2296,6 +2552,9 @@
       <c r="E22" t="s">
         <v>105</v>
       </c>
+      <c r="F22" t="s">
+        <v>338</v>
+      </c>
       <c r="G22">
         <v>109.95</v>
       </c>
@@ -2337,6 +2596,9 @@
       <c r="E23" t="s">
         <v>108</v>
       </c>
+      <c r="F23" t="s">
+        <v>339</v>
+      </c>
       <c r="H23">
         <v>74.95</v>
       </c>
@@ -2378,6 +2640,9 @@
       <c r="E24" t="s">
         <v>112</v>
       </c>
+      <c r="F24" t="s">
+        <v>340</v>
+      </c>
       <c r="G24">
         <v>64.95</v>
       </c>
@@ -2419,6 +2684,9 @@
       <c r="E25" t="s">
         <v>117</v>
       </c>
+      <c r="F25" t="s">
+        <v>341</v>
+      </c>
       <c r="H25">
         <v>179.95</v>
       </c>
@@ -2454,6 +2722,9 @@
       <c r="E26" t="s">
         <v>118</v>
       </c>
+      <c r="F26" t="s">
+        <v>342</v>
+      </c>
       <c r="G26">
         <v>69.95</v>
       </c>
@@ -2492,6 +2763,9 @@
       <c r="E27" t="s">
         <v>124</v>
       </c>
+      <c r="F27" t="s">
+        <v>343</v>
+      </c>
       <c r="G27">
         <v>149.94999999999999</v>
       </c>
@@ -2568,6 +2842,9 @@
       <c r="E29" t="s">
         <v>137</v>
       </c>
+      <c r="F29" t="s">
+        <v>344</v>
+      </c>
       <c r="G29">
         <v>99.95</v>
       </c>
@@ -2606,6 +2883,9 @@
       <c r="E30" t="s">
         <v>135</v>
       </c>
+      <c r="F30" t="s">
+        <v>345</v>
+      </c>
       <c r="G30">
         <v>279.95</v>
       </c>
@@ -2682,6 +2962,9 @@
       <c r="E32" t="s">
         <v>144</v>
       </c>
+      <c r="F32" t="s">
+        <v>317</v>
+      </c>
       <c r="H32">
         <v>249</v>
       </c>
@@ -2717,6 +3000,9 @@
       <c r="E33" t="s">
         <v>147</v>
       </c>
+      <c r="F33" t="s">
+        <v>346</v>
+      </c>
       <c r="G33">
         <v>144.94999999999999</v>
       </c>
@@ -2831,6 +3117,9 @@
       <c r="E36" t="s">
         <v>154</v>
       </c>
+      <c r="F36" t="s">
+        <v>347</v>
+      </c>
       <c r="G36">
         <v>99.95</v>
       </c>
@@ -3082,6 +3371,9 @@
       <c r="E43" t="s">
         <v>169</v>
       </c>
+      <c r="F43" t="s">
+        <v>304</v>
+      </c>
       <c r="H43">
         <v>49.95</v>
       </c>
@@ -3120,6 +3412,9 @@
       <c r="E44" t="s">
         <v>173</v>
       </c>
+      <c r="F44" t="s">
+        <v>305</v>
+      </c>
       <c r="H44">
         <v>29.95</v>
       </c>
@@ -3161,6 +3456,9 @@
       <c r="E45" t="s">
         <v>300</v>
       </c>
+      <c r="F45" t="s">
+        <v>306</v>
+      </c>
       <c r="G45">
         <v>129.94999999999999</v>
       </c>
@@ -3231,6 +3529,9 @@
       <c r="E47" t="s">
         <v>179</v>
       </c>
+      <c r="F47" t="s">
+        <v>307</v>
+      </c>
       <c r="H47">
         <v>399.95</v>
       </c>
@@ -3269,6 +3570,9 @@
       <c r="E48" t="s">
         <v>180</v>
       </c>
+      <c r="F48" t="s">
+        <v>308</v>
+      </c>
       <c r="H48">
         <v>159.94999999999999</v>
       </c>
@@ -3307,6 +3611,9 @@
       <c r="E49" t="s">
         <v>182</v>
       </c>
+      <c r="F49" t="s">
+        <v>309</v>
+      </c>
       <c r="H49">
         <v>149.94999999999999</v>
       </c>
@@ -3345,6 +3652,9 @@
       <c r="E50" t="s">
         <v>187</v>
       </c>
+      <c r="F50" t="s">
+        <v>310</v>
+      </c>
       <c r="H50">
         <v>129.94999999999999</v>
       </c>
@@ -3383,6 +3693,9 @@
       <c r="E51" t="s">
         <v>190</v>
       </c>
+      <c r="F51" t="s">
+        <v>311</v>
+      </c>
       <c r="H51">
         <v>79.95</v>
       </c>
@@ -3503,6 +3816,9 @@
       <c r="E54" t="s">
         <v>200</v>
       </c>
+      <c r="F54" t="s">
+        <v>312</v>
+      </c>
       <c r="G54">
         <v>49.95</v>
       </c>
@@ -3582,6 +3898,9 @@
       <c r="E56" t="s">
         <v>302</v>
       </c>
+      <c r="F56" t="s">
+        <v>313</v>
+      </c>
       <c r="G56">
         <v>24.95</v>
       </c>
@@ -3620,6 +3939,9 @@
       <c r="E57" t="s">
         <v>208</v>
       </c>
+      <c r="F57" t="s">
+        <v>314</v>
+      </c>
       <c r="G57">
         <v>39.950000000000003</v>
       </c>
@@ -3661,6 +3983,9 @@
       <c r="E58" t="s">
         <v>210</v>
       </c>
+      <c r="F58" t="s">
+        <v>315</v>
+      </c>
       <c r="G58">
         <v>99.95</v>
       </c>
@@ -3702,6 +4027,9 @@
       <c r="E59" t="s">
         <v>213</v>
       </c>
+      <c r="F59" t="s">
+        <v>316</v>
+      </c>
       <c r="H59">
         <v>29.95</v>
       </c>
@@ -3740,6 +4068,9 @@
       <c r="E60" t="s">
         <v>144</v>
       </c>
+      <c r="F60" t="s">
+        <v>317</v>
+      </c>
       <c r="H60">
         <v>169</v>
       </c>
@@ -3778,6 +4109,9 @@
       <c r="E61" t="s">
         <v>303</v>
       </c>
+      <c r="F61" t="s">
+        <v>318</v>
+      </c>
       <c r="H61" s="1">
         <v>1299</v>
       </c>
@@ -3813,6 +4147,9 @@
       <c r="D62" t="s">
         <v>221</v>
       </c>
+      <c r="E62" t="s">
+        <v>349</v>
+      </c>
       <c r="H62">
         <v>69.95</v>
       </c>
@@ -3851,6 +4188,9 @@
       <c r="E63" t="s">
         <v>225</v>
       </c>
+      <c r="F63" t="s">
+        <v>319</v>
+      </c>
       <c r="G63">
         <v>74.95</v>
       </c>
@@ -3886,6 +4226,9 @@
       <c r="E64" t="s">
         <v>228</v>
       </c>
+      <c r="F64" t="s">
+        <v>320</v>
+      </c>
       <c r="G64">
         <v>149.94999999999999</v>
       </c>
@@ -3921,6 +4264,12 @@
       <c r="D65" t="s">
         <v>293</v>
       </c>
+      <c r="E65" t="s">
+        <v>348</v>
+      </c>
+      <c r="F65" t="s">
+        <v>321</v>
+      </c>
       <c r="G65">
         <v>149.94999999999999</v>
       </c>
@@ -3953,6 +4302,12 @@
       <c r="D66" t="s">
         <v>127</v>
       </c>
+      <c r="E66" t="s">
+        <v>350</v>
+      </c>
+      <c r="F66" t="s">
+        <v>322</v>
+      </c>
       <c r="H66">
         <v>74.95</v>
       </c>
@@ -3988,6 +4343,9 @@
       <c r="D67" t="s">
         <v>234</v>
       </c>
+      <c r="E67" t="s">
+        <v>351</v>
+      </c>
       <c r="H67">
         <v>24.95</v>
       </c>
@@ -4020,8 +4378,14 @@
       <c r="D68" t="s">
         <v>240</v>
       </c>
+      <c r="E68" t="s">
+        <v>352</v>
+      </c>
       <c r="H68">
         <v>29.95</v>
+      </c>
+      <c r="I68" t="s">
+        <v>353</v>
       </c>
       <c r="N68">
         <v>33</v>
@@ -4046,6 +4410,9 @@
       <c r="D69" t="s">
         <v>242</v>
       </c>
+      <c r="E69" t="s">
+        <v>354</v>
+      </c>
       <c r="H69">
         <v>19.95</v>
       </c>
@@ -4072,6 +4439,9 @@
       <c r="D70" t="s">
         <v>240</v>
       </c>
+      <c r="E70" t="s">
+        <v>355</v>
+      </c>
       <c r="H70">
         <v>24.95</v>
       </c>
@@ -4098,6 +4468,9 @@
       <c r="D71" t="s">
         <v>240</v>
       </c>
+      <c r="E71" t="s">
+        <v>356</v>
+      </c>
       <c r="H71">
         <v>24.95</v>
       </c>
@@ -4124,6 +4497,9 @@
       <c r="D72" t="s">
         <v>240</v>
       </c>
+      <c r="E72" t="s">
+        <v>357</v>
+      </c>
       <c r="H72">
         <v>24.95</v>
       </c>
@@ -4150,6 +4526,9 @@
       <c r="D73" t="s">
         <v>242</v>
       </c>
+      <c r="E73" t="s">
+        <v>358</v>
+      </c>
       <c r="H73">
         <v>19.95</v>
       </c>
@@ -4176,6 +4555,9 @@
       <c r="D74" t="s">
         <v>242</v>
       </c>
+      <c r="E74" t="s">
+        <v>359</v>
+      </c>
       <c r="H74">
         <v>29.95</v>
       </c>
@@ -4202,6 +4584,9 @@
       <c r="D75" t="s">
         <v>242</v>
       </c>
+      <c r="E75" t="s">
+        <v>360</v>
+      </c>
       <c r="H75">
         <v>24.95</v>
       </c>
@@ -4231,6 +4616,12 @@
       <c r="D76" t="s">
         <v>141</v>
       </c>
+      <c r="E76" t="s">
+        <v>361</v>
+      </c>
+      <c r="F76" t="s">
+        <v>323</v>
+      </c>
       <c r="H76">
         <v>449</v>
       </c>
@@ -4257,6 +4648,9 @@
       <c r="D77" t="s">
         <v>240</v>
       </c>
+      <c r="E77" t="s">
+        <v>362</v>
+      </c>
       <c r="H77">
         <v>19.95</v>
       </c>
@@ -4283,6 +4677,9 @@
       <c r="D78" t="s">
         <v>240</v>
       </c>
+      <c r="E78" t="s">
+        <v>363</v>
+      </c>
       <c r="H78">
         <v>19.95</v>
       </c>
@@ -4312,6 +4709,12 @@
       <c r="D79" t="s">
         <v>254</v>
       </c>
+      <c r="E79" t="s">
+        <v>364</v>
+      </c>
+      <c r="F79" t="s">
+        <v>324</v>
+      </c>
       <c r="H79">
         <v>59.95</v>
       </c>
@@ -4340,6 +4743,9 @@
       </c>
       <c r="D80" t="s">
         <v>256</v>
+      </c>
+      <c r="E80" t="s">
+        <v>365</v>
       </c>
       <c r="R80">
         <v>40</v>

</xml_diff>

<commit_message>
Packshots & excel aangepast
</commit_message>
<xml_diff>
--- a/excel/producten.xlsx
+++ b/excel/producten.xlsx
@@ -720,9 +720,6 @@
     <t>Blowy</t>
   </si>
   <si>
-    <t>RH+_BLOWY-JACKET_9221d42011_7070_01_be.jpg</t>
-  </si>
-  <si>
     <t>#252525</t>
   </si>
   <si>
@@ -1122,9 +1119,6 @@
     <t>LEZYNE_MACRO-DRIVE-600_A372C52002_7070.jpg</t>
   </si>
   <si>
-    <t>VAUDE_FLUID-II_7745b80004_7070_01.jpg</t>
-  </si>
-  <si>
     <t>Contigo-packshot.jpg</t>
   </si>
   <si>
@@ -1168,6 +1162,12 @@
   </si>
   <si>
     <t>TOMTOM_RUNNER2CARDIO+MUSIC_.jpg</t>
+  </si>
+  <si>
+    <t>VAUDEFLUIDII7745b80004707001.jpg</t>
+  </si>
+  <si>
+    <t>RHBLOWYJACKET9221d42011707001be.jpg</t>
   </si>
 </sst>
 </file>
@@ -1251,16 +1251,16 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="21">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1271,7 +1271,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1607,10 +1607,10 @@
   <dimension ref="A1:W80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="37" topLeftCell="K38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="37" topLeftCell="K44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
-      <selection pane="bottomRight" activeCell="E82" sqref="E82"/>
+      <selection pane="bottomRight" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1719,7 +1719,7 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -1760,7 +1760,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -1769,7 +1769,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G3">
         <v>89.95</v>
@@ -1814,7 +1814,7 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G4">
         <v>79.989999999999995</v>
@@ -1858,7 +1858,7 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G5">
         <v>79.989999999999995</v>
@@ -1893,7 +1893,7 @@
         <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
@@ -1902,7 +1902,7 @@
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G6">
         <v>69.989999999999995</v>
@@ -1944,10 +1944,10 @@
         <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H7">
         <v>99.95</v>
@@ -1994,7 +1994,7 @@
         <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H8">
         <v>8.9499999999999993</v>
@@ -2026,7 +2026,7 @@
         <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
         <v>53</v>
@@ -2035,7 +2035,7 @@
         <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H9">
         <v>49.99</v>
@@ -2102,7 +2102,7 @@
         <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D11" t="s">
         <v>62</v>
@@ -2111,7 +2111,7 @@
         <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G11">
         <v>69.95</v>
@@ -2143,7 +2143,7 @@
         <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D12" t="s">
         <v>66</v>
@@ -2152,7 +2152,7 @@
         <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G12">
         <v>149</v>
@@ -2187,7 +2187,7 @@
         <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D13" t="s">
         <v>70</v>
@@ -2196,7 +2196,7 @@
         <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H13">
         <v>499.95</v>
@@ -2234,7 +2234,7 @@
         <v>75</v>
       </c>
       <c r="F14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G14">
         <v>49.95</v>
@@ -2272,7 +2272,7 @@
         <v>78</v>
       </c>
       <c r="E15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H15">
         <v>124.95</v>
@@ -2348,7 +2348,7 @@
         <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D17" t="s">
         <v>86</v>
@@ -2386,7 +2386,7 @@
         <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D18" t="s">
         <v>86</v>
@@ -2424,7 +2424,7 @@
         <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D19" t="s">
         <v>94</v>
@@ -2433,7 +2433,7 @@
         <v>95</v>
       </c>
       <c r="F19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H19">
         <v>169.95</v>
@@ -2465,7 +2465,7 @@
         <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D20" t="s">
         <v>94</v>
@@ -2503,7 +2503,7 @@
         <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D21" t="s">
         <v>94</v>
@@ -2512,7 +2512,7 @@
         <v>100</v>
       </c>
       <c r="F21" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G21">
         <v>59.95</v>
@@ -2553,7 +2553,7 @@
         <v>105</v>
       </c>
       <c r="F22" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G22">
         <v>109.95</v>
@@ -2588,7 +2588,7 @@
         <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D23" t="s">
         <v>94</v>
@@ -2597,7 +2597,7 @@
         <v>108</v>
       </c>
       <c r="F23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H23">
         <v>74.95</v>
@@ -2641,7 +2641,7 @@
         <v>112</v>
       </c>
       <c r="F24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G24">
         <v>64.95</v>
@@ -2685,7 +2685,7 @@
         <v>117</v>
       </c>
       <c r="F25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H25">
         <v>179.95</v>
@@ -2714,7 +2714,7 @@
         <v>120</v>
       </c>
       <c r="C26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D26" t="s">
         <v>121</v>
@@ -2723,7 +2723,7 @@
         <v>118</v>
       </c>
       <c r="F26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G26">
         <v>69.95</v>
@@ -2755,7 +2755,7 @@
         <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D27" t="s">
         <v>121</v>
@@ -2764,7 +2764,7 @@
         <v>124</v>
       </c>
       <c r="F27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G27">
         <v>149.94999999999999</v>
@@ -2796,7 +2796,7 @@
         <v>126</v>
       </c>
       <c r="C28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D28" t="s">
         <v>127</v>
@@ -2834,7 +2834,7 @@
         <v>131</v>
       </c>
       <c r="C29" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D29" t="s">
         <v>130</v>
@@ -2843,7 +2843,7 @@
         <v>137</v>
       </c>
       <c r="F29" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G29">
         <v>99.95</v>
@@ -2875,7 +2875,7 @@
         <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D30" t="s">
         <v>134</v>
@@ -2884,7 +2884,7 @@
         <v>135</v>
       </c>
       <c r="F30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G30">
         <v>279.95</v>
@@ -2916,7 +2916,7 @@
         <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D31" t="s">
         <v>121</v>
@@ -2963,7 +2963,7 @@
         <v>144</v>
       </c>
       <c r="F32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H32">
         <v>249</v>
@@ -3001,7 +3001,7 @@
         <v>147</v>
       </c>
       <c r="F33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G33">
         <v>144.94999999999999</v>
@@ -3036,13 +3036,13 @@
         <v>148</v>
       </c>
       <c r="C34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D34" t="s">
         <v>127</v>
       </c>
       <c r="E34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G34">
         <v>99.95</v>
@@ -3071,7 +3071,7 @@
         <v>149</v>
       </c>
       <c r="C35" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D35" t="s">
         <v>81</v>
@@ -3109,7 +3109,7 @@
         <v>152</v>
       </c>
       <c r="C36" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D36" t="s">
         <v>81</v>
@@ -3118,7 +3118,7 @@
         <v>154</v>
       </c>
       <c r="F36" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G36">
         <v>99.95</v>
@@ -3150,13 +3150,13 @@
         <v>156</v>
       </c>
       <c r="C37" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D37" t="s">
         <v>155</v>
       </c>
       <c r="E37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G37">
         <v>119.95</v>
@@ -3185,13 +3185,13 @@
         <v>156</v>
       </c>
       <c r="C38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D38" t="s">
         <v>155</v>
       </c>
       <c r="E38" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G38">
         <v>119.95</v>
@@ -3220,7 +3220,7 @@
         <v>157</v>
       </c>
       <c r="C39" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D39" t="s">
         <v>155</v>
@@ -3258,7 +3258,7 @@
         <v>160</v>
       </c>
       <c r="C40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D40" t="s">
         <v>155</v>
@@ -3296,13 +3296,13 @@
         <v>163</v>
       </c>
       <c r="C41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D41" t="s">
         <v>155</v>
       </c>
       <c r="E41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G41">
         <v>199.95</v>
@@ -3331,13 +3331,19 @@
         <v>164</v>
       </c>
       <c r="C42" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D42" t="s">
         <v>155</v>
       </c>
       <c r="E42" t="s">
         <v>165</v>
+      </c>
+      <c r="G42">
+        <v>279.95</v>
+      </c>
+      <c r="H42">
+        <v>199</v>
       </c>
       <c r="I42" t="s">
         <v>166</v>
@@ -3372,7 +3378,7 @@
         <v>169</v>
       </c>
       <c r="F43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H43">
         <v>49.95</v>
@@ -3413,7 +3419,7 @@
         <v>173</v>
       </c>
       <c r="F44" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H44">
         <v>29.95</v>
@@ -3448,16 +3454,16 @@
         <v>176</v>
       </c>
       <c r="C45" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D45" t="s">
         <v>175</v>
       </c>
       <c r="E45" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G45">
         <v>129.94999999999999</v>
@@ -3486,13 +3492,13 @@
         <v>176</v>
       </c>
       <c r="C46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D46" t="s">
         <v>175</v>
       </c>
       <c r="E46" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G46">
         <v>129.94999999999999</v>
@@ -3521,7 +3527,7 @@
         <v>177</v>
       </c>
       <c r="C47" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D47" t="s">
         <v>70</v>
@@ -3530,7 +3536,7 @@
         <v>179</v>
       </c>
       <c r="F47" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H47">
         <v>399.95</v>
@@ -3562,7 +3568,7 @@
         <v>178</v>
       </c>
       <c r="C48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D48" t="s">
         <v>70</v>
@@ -3571,7 +3577,7 @@
         <v>180</v>
       </c>
       <c r="F48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H48">
         <v>159.94999999999999</v>
@@ -3603,7 +3609,7 @@
         <v>181</v>
       </c>
       <c r="C49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D49" t="s">
         <v>70</v>
@@ -3612,13 +3618,13 @@
         <v>182</v>
       </c>
       <c r="F49" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H49">
         <v>149.94999999999999</v>
       </c>
       <c r="I49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J49" t="s">
         <v>45</v>
@@ -3644,7 +3650,7 @@
         <v>185</v>
       </c>
       <c r="C50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D50" t="s">
         <v>70</v>
@@ -3653,13 +3659,13 @@
         <v>187</v>
       </c>
       <c r="F50" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H50">
         <v>129.94999999999999</v>
       </c>
       <c r="I50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J50" t="s">
         <v>45</v>
@@ -3694,7 +3700,7 @@
         <v>190</v>
       </c>
       <c r="F51" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H51">
         <v>79.95</v>
@@ -3759,7 +3765,7 @@
         <v>43</v>
       </c>
       <c r="U52" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V52">
         <v>151</v>
@@ -3773,7 +3779,7 @@
         <v>196</v>
       </c>
       <c r="C53" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D53" t="s">
         <v>192</v>
@@ -3794,7 +3800,7 @@
         <v>46</v>
       </c>
       <c r="U53" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V53">
         <v>154</v>
@@ -3808,7 +3814,7 @@
         <v>198</v>
       </c>
       <c r="C54" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D54" t="s">
         <v>199</v>
@@ -3817,7 +3823,7 @@
         <v>200</v>
       </c>
       <c r="F54" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G54">
         <v>49.95</v>
@@ -3835,7 +3841,7 @@
         <v>49</v>
       </c>
       <c r="U54" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V54">
         <v>157</v>
@@ -3849,7 +3855,7 @@
         <v>202</v>
       </c>
       <c r="C55" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D55" t="s">
         <v>23</v>
@@ -3876,7 +3882,7 @@
         <v>52</v>
       </c>
       <c r="U55" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V55">
         <v>160</v>
@@ -3890,16 +3896,16 @@
         <v>205</v>
       </c>
       <c r="C56" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D56" t="s">
         <v>206</v>
       </c>
       <c r="E56" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G56">
         <v>24.95</v>
@@ -3917,7 +3923,7 @@
         <v>55</v>
       </c>
       <c r="U56" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V56">
         <v>163</v>
@@ -3931,7 +3937,7 @@
         <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D57" t="s">
         <v>207</v>
@@ -3940,7 +3946,7 @@
         <v>208</v>
       </c>
       <c r="F57" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G57">
         <v>39.950000000000003</v>
@@ -3961,7 +3967,7 @@
         <v>58</v>
       </c>
       <c r="U57" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V57">
         <v>166</v>
@@ -3975,7 +3981,7 @@
         <v>209</v>
       </c>
       <c r="C58" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D58" t="s">
         <v>155</v>
@@ -3984,7 +3990,7 @@
         <v>210</v>
       </c>
       <c r="F58" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G58">
         <v>99.95</v>
@@ -4005,7 +4011,7 @@
         <v>80</v>
       </c>
       <c r="U58" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V58">
         <v>169</v>
@@ -4019,7 +4025,7 @@
         <v>212</v>
       </c>
       <c r="C59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D59" t="s">
         <v>155</v>
@@ -4028,7 +4034,7 @@
         <v>213</v>
       </c>
       <c r="F59" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H59">
         <v>29.95</v>
@@ -4046,7 +4052,7 @@
         <v>27</v>
       </c>
       <c r="U59" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V59">
         <v>172</v>
@@ -4069,7 +4075,7 @@
         <v>144</v>
       </c>
       <c r="F60" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H60">
         <v>169</v>
@@ -4101,22 +4107,22 @@
         <v>217</v>
       </c>
       <c r="C61" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D61" t="s">
         <v>218</v>
       </c>
       <c r="E61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F61" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H61" s="1">
         <v>1299</v>
       </c>
       <c r="J61" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N61">
         <v>201</v>
@@ -4148,7 +4154,7 @@
         <v>221</v>
       </c>
       <c r="E62" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H62">
         <v>69.95</v>
@@ -4189,7 +4195,7 @@
         <v>225</v>
       </c>
       <c r="F63" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G63">
         <v>74.95</v>
@@ -4198,7 +4204,7 @@
         <v>59</v>
       </c>
       <c r="I63" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="S63">
         <v>7</v>
@@ -4218,16 +4224,16 @@
         <v>227</v>
       </c>
       <c r="C64" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D64" t="s">
         <v>226</v>
       </c>
       <c r="E64" t="s">
-        <v>228</v>
+        <v>365</v>
       </c>
       <c r="F64" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G64">
         <v>149.94999999999999</v>
@@ -4236,7 +4242,7 @@
         <v>99</v>
       </c>
       <c r="I64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N64">
         <v>205</v>
@@ -4256,19 +4262,19 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D65" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E65" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F65" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G65">
         <v>149.94999999999999</v>
@@ -4294,7 +4300,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C66" t="s">
         <v>186</v>
@@ -4303,10 +4309,10 @@
         <v>127</v>
       </c>
       <c r="E66" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="F66" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H66">
         <v>74.95</v>
@@ -4335,22 +4341,22 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D67" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E67" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H67">
         <v>24.95</v>
       </c>
       <c r="J67" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N67">
         <v>30</v>
@@ -4370,22 +4376,22 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>238</v>
+      </c>
+      <c r="C68" t="s">
+        <v>237</v>
+      </c>
+      <c r="D68" t="s">
         <v>239</v>
       </c>
-      <c r="C68" t="s">
-        <v>238</v>
-      </c>
-      <c r="D68" t="s">
-        <v>240</v>
-      </c>
       <c r="E68" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H68">
         <v>29.95</v>
       </c>
       <c r="I68" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N68">
         <v>33</v>
@@ -4405,13 +4411,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>240</v>
+      </c>
+      <c r="D69" t="s">
         <v>241</v>
       </c>
-      <c r="D69" t="s">
-        <v>242</v>
-      </c>
       <c r="E69" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H69">
         <v>19.95</v>
@@ -4434,13 +4440,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D70" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E70" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H70">
         <v>24.95</v>
@@ -4463,13 +4469,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D71" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E71" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H71">
         <v>24.95</v>
@@ -4492,13 +4498,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D72" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E72" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H72">
         <v>24.95</v>
@@ -4521,13 +4527,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D73" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E73" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H73">
         <v>19.95</v>
@@ -4550,13 +4556,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D74" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E74" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H74">
         <v>29.95</v>
@@ -4579,13 +4585,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D75" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E75" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H75">
         <v>24.95</v>
@@ -4608,19 +4614,19 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C76" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D76" t="s">
         <v>141</v>
       </c>
       <c r="E76" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F76" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H76">
         <v>449</v>
@@ -4643,13 +4649,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D77" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E77" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H77">
         <v>19.95</v>
@@ -4672,13 +4678,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D78" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E78" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H78">
         <v>19.95</v>
@@ -4701,19 +4707,19 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>252</v>
+      </c>
+      <c r="C79" t="s">
+        <v>254</v>
+      </c>
+      <c r="D79" t="s">
         <v>253</v>
       </c>
-      <c r="C79" t="s">
-        <v>255</v>
-      </c>
-      <c r="D79" t="s">
-        <v>254</v>
-      </c>
       <c r="E79" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F79" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H79">
         <v>59.95</v>
@@ -4736,16 +4742,19 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C80" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E80" t="s">
-        <v>365</v>
+        <v>363</v>
+      </c>
+      <c r="H80">
+        <v>199.95</v>
       </c>
       <c r="R80">
         <v>40</v>

</xml_diff>

<commit_message>
bijvoegen swatches en productlinken
</commit_message>
<xml_diff>
--- a/excel/producten.xlsx
+++ b/excel/producten.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40980" windowHeight="25260" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="26600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="producten.csv" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="386">
   <si>
     <t>id</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>CKS_JAQUELINEA_4141D52036_5252.jpg</t>
-  </si>
-  <si>
-    <t>#4C5059 marmer.jpg</t>
   </si>
   <si>
     <t>Balance</t>
@@ -732,6 +729,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t>#8A7D75</t>
@@ -1169,6 +1167,69 @@
   <si>
     <t>RHBLOWYJACKET9221d42011707001be.jpg</t>
   </si>
+  <si>
+    <t>/cks-dames-blazer-jaquelinea-4141d52036?id_colour=3154</t>
+  </si>
+  <si>
+    <t>/dstrezzed-hemd-300001137smu-4331d52232?id_colour=2728</t>
+  </si>
+  <si>
+    <t>/ray-ban-bril-rb2132-2412a82013?id_colour=3700</t>
+  </si>
+  <si>
+    <t>/the-north-face-dagrugzak-borealis-classic-2111d50014?id_colour=4169</t>
+  </si>
+  <si>
+    <t>/cks-kids-broek-roja-5291d52031?id_colour=366</t>
+  </si>
+  <si>
+    <t>/someone-hemd-checkmate-5331d52026?id_colour=2287</t>
+  </si>
+  <si>
+    <t>/someone-trui-funny-bunny-5244d52014?id_colour=346</t>
+  </si>
+  <si>
+    <t>/lowa-schoen-palermo-gore-tex-3712d52001?id_colour=3565</t>
+  </si>
+  <si>
+    <t>/jack-wolfskin-jas-stenton-3351d52014?id_colour=4168</t>
+  </si>
+  <si>
+    <t>/jack-wolfskin-jas-crush-n-ice-3151d32005?id_colour=2842</t>
+  </si>
+  <si>
+    <t>/jack-wolfskin-fleece-caribou-3324d52018?id_colour=2296</t>
+  </si>
+  <si>
+    <t>/jack-wolfskin-fleece-peridot-3124d52010?id_colour=1594</t>
+  </si>
+  <si>
+    <t>/jack-wolfskin-jas-madison-3353d52013?id_colour=4246</t>
+  </si>
+  <si>
+    <t>/jack-wolfskin-jas-madison-3153d52011?id_colour=2296</t>
+  </si>
+  <si>
+    <t>/vaude-fleece-bronia-3124d52007?id_colour=4324</t>
+  </si>
+  <si>
+    <t>/sprayway-fleece-heritage-3324d42017?id_colour=2296</t>
+  </si>
+  <si>
+    <t>/vaude-jas-limford-3353d32003?id_colour=2296</t>
+  </si>
+  <si>
+    <t>/ayacucho-trui-nordic-wood-3325d52007?id_colour=3544</t>
+  </si>
+  <si>
+    <t>marmer.jpg</t>
+  </si>
+  <si>
+    <t>rayban.jpg</t>
+  </si>
+  <si>
+    <t>ayacucho-sneeuw.jpg</t>
+  </si>
 </sst>
 </file>
 
@@ -1180,6 +1241,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1607,10 +1669,10 @@
   <dimension ref="A1:W80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="37" topLeftCell="K44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="37" topLeftCell="I38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
-      <selection pane="bottomRight" activeCell="E64" sqref="E64"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1619,7 +1681,7 @@
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" customWidth="1"/>
+    <col min="5" max="5" width="56.5" customWidth="1"/>
     <col min="6" max="6" width="54.83203125" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -1719,13 +1781,16 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>365</v>
       </c>
       <c r="G2">
         <v>79.989999999999995</v>
@@ -1760,7 +1825,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -1769,7 +1834,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G3">
         <v>89.95</v>
@@ -1778,7 +1843,7 @@
         <v>59</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>383</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1802,19 +1867,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G4">
         <v>79.989999999999995</v>
@@ -1823,7 +1888,7 @@
         <v>55</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1846,19 +1911,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
       <c r="F5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G5">
         <v>79.989999999999995</v>
@@ -1867,7 +1932,7 @@
         <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -1890,19 +1955,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
       <c r="F6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G6">
         <v>69.989999999999995</v>
@@ -1911,7 +1976,7 @@
         <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1935,28 +2000,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
       <c r="E7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H7">
         <v>99.95</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M7">
         <v>15</v>
@@ -1982,28 +2047,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>49</v>
       </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
       <c r="F8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H8">
         <v>8.9499999999999993</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M8">
         <v>17</v>
@@ -2023,28 +2088,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
-        <v>260</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>53</v>
       </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
       <c r="F9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H9">
         <v>49.99</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N9">
         <v>5</v>
@@ -2064,13 +2129,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
-        <v>59</v>
+      <c r="F10" t="s">
+        <v>366</v>
       </c>
       <c r="G10">
         <v>79.95</v>
@@ -2079,7 +2147,7 @@
         <v>49</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N10">
         <v>7</v>
@@ -2099,19 +2167,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D11" t="s">
         <v>61</v>
       </c>
-      <c r="C11" t="s">
-        <v>261</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>62</v>
       </c>
-      <c r="E11" t="s">
-        <v>63</v>
-      </c>
       <c r="F11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G11">
         <v>69.95</v>
@@ -2120,7 +2188,7 @@
         <v>49</v>
       </c>
       <c r="I11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N11">
         <v>10</v>
@@ -2140,19 +2208,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
-        <v>262</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>66</v>
       </c>
-      <c r="E12" t="s">
-        <v>67</v>
-      </c>
       <c r="F12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G12">
         <v>149</v>
@@ -2161,7 +2229,7 @@
         <v>99</v>
       </c>
       <c r="I12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -2184,25 +2252,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D13" t="s">
         <v>69</v>
       </c>
-      <c r="C13" t="s">
-        <v>263</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>70</v>
       </c>
-      <c r="E13" t="s">
-        <v>71</v>
-      </c>
       <c r="F13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H13">
         <v>499.95</v>
       </c>
       <c r="I13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N13">
         <v>100</v>
@@ -2225,16 +2293,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
         <v>73</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>74</v>
       </c>
-      <c r="E14" t="s">
-        <v>75</v>
-      </c>
       <c r="F14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G14">
         <v>49.95</v>
@@ -2243,7 +2311,7 @@
         <v>25</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N14">
         <v>15</v>
@@ -2266,19 +2334,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" t="s">
         <v>77</v>
       </c>
-      <c r="D15" t="s">
-        <v>78</v>
-      </c>
       <c r="E15" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="F15" t="s">
+        <v>367</v>
       </c>
       <c r="H15">
         <v>124.95</v>
       </c>
+      <c r="I15" t="s">
+        <v>384</v>
+      </c>
       <c r="J15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M15">
         <v>22</v>
@@ -2304,16 +2378,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
         <v>80</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>82</v>
       </c>
-      <c r="D16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" t="s">
-        <v>83</v>
+      <c r="F16" t="s">
+        <v>368</v>
       </c>
       <c r="G16">
         <v>79.95</v>
@@ -2322,7 +2399,7 @@
         <v>59</v>
       </c>
       <c r="I16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M16">
         <v>102</v>
@@ -2345,16 +2422,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>263</v>
+      </c>
+      <c r="D17" t="s">
         <v>85</v>
       </c>
-      <c r="C17" t="s">
-        <v>264</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>86</v>
-      </c>
-      <c r="E17" t="s">
-        <v>87</v>
       </c>
       <c r="G17">
         <v>119.95</v>
@@ -2363,7 +2440,7 @@
         <v>85</v>
       </c>
       <c r="I17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M17">
         <v>105</v>
@@ -2372,7 +2449,7 @@
         <v>3</v>
       </c>
       <c r="U17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V17">
         <v>46</v>
@@ -2383,16 +2460,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
         <v>89</v>
-      </c>
-      <c r="C18" t="s">
-        <v>265</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>90</v>
       </c>
       <c r="G18">
         <v>125.95</v>
@@ -2401,7 +2478,7 @@
         <v>89</v>
       </c>
       <c r="I18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N18">
         <v>103</v>
@@ -2410,7 +2487,7 @@
         <v>6</v>
       </c>
       <c r="U18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V18">
         <v>49</v>
@@ -2421,28 +2498,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" t="s">
+        <v>265</v>
+      </c>
+      <c r="D19" t="s">
         <v>93</v>
       </c>
-      <c r="C19" t="s">
-        <v>266</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>94</v>
       </c>
-      <c r="E19" t="s">
-        <v>95</v>
-      </c>
       <c r="F19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H19">
         <v>169.95</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N19">
         <v>106</v>
@@ -2451,7 +2528,7 @@
         <v>9</v>
       </c>
       <c r="U19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V19">
         <v>52</v>
@@ -2462,22 +2539,28 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>266</v>
+      </c>
+      <c r="D20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" t="s">
         <v>97</v>
       </c>
-      <c r="C20" t="s">
-        <v>267</v>
-      </c>
-      <c r="D20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" t="s">
-        <v>98</v>
+      <c r="F20" t="s">
+        <v>382</v>
       </c>
       <c r="H20">
         <v>69.95</v>
       </c>
+      <c r="I20" t="s">
+        <v>385</v>
+      </c>
       <c r="J20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N20">
         <v>107</v>
@@ -2489,7 +2572,7 @@
         <v>12</v>
       </c>
       <c r="U20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V20">
         <v>55</v>
@@ -2500,19 +2583,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" t="s">
+        <v>267</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" t="s">
         <v>99</v>
       </c>
-      <c r="C21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D21" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" t="s">
-        <v>100</v>
-      </c>
       <c r="F21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G21">
         <v>59.95</v>
@@ -2521,7 +2604,7 @@
         <v>39.950000000000003</v>
       </c>
       <c r="I21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M21">
         <v>108</v>
@@ -2530,7 +2613,7 @@
         <v>15</v>
       </c>
       <c r="U21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V21">
         <v>58</v>
@@ -2541,19 +2624,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" t="s">
         <v>102</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>103</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>104</v>
       </c>
-      <c r="E22" t="s">
-        <v>105</v>
-      </c>
       <c r="F22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G22">
         <v>109.95</v>
@@ -2562,7 +2645,7 @@
         <v>75</v>
       </c>
       <c r="I22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M22">
         <v>111</v>
@@ -2574,7 +2657,7 @@
         <v>3</v>
       </c>
       <c r="U22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V22">
         <v>61</v>
@@ -2585,28 +2668,28 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" t="s">
+        <v>268</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" t="s">
         <v>107</v>
       </c>
-      <c r="C23" t="s">
-        <v>269</v>
-      </c>
-      <c r="D23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" t="s">
-        <v>108</v>
-      </c>
       <c r="F23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H23">
         <v>74.95</v>
       </c>
       <c r="I23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M23">
         <v>115</v>
@@ -2618,7 +2701,7 @@
         <v>21</v>
       </c>
       <c r="U23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V23">
         <v>64</v>
@@ -2629,19 +2712,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
         <v>110</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" t="s">
         <v>111</v>
       </c>
-      <c r="D24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" t="s">
-        <v>112</v>
-      </c>
       <c r="F24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G24">
         <v>64.95</v>
@@ -2650,7 +2733,7 @@
         <v>39</v>
       </c>
       <c r="I24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M24">
         <v>118</v>
@@ -2662,7 +2745,7 @@
         <v>6</v>
       </c>
       <c r="U24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V24">
         <v>67</v>
@@ -2673,25 +2756,25 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" t="s">
         <v>114</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>115</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>116</v>
       </c>
-      <c r="E25" t="s">
-        <v>117</v>
-      </c>
       <c r="F25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H25">
         <v>179.95</v>
       </c>
       <c r="I25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R25">
         <v>9</v>
@@ -2700,7 +2783,7 @@
         <v>10</v>
       </c>
       <c r="U25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V25">
         <v>70</v>
@@ -2711,19 +2794,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" t="s">
+        <v>267</v>
+      </c>
+      <c r="D26" t="s">
         <v>120</v>
       </c>
-      <c r="C26" t="s">
-        <v>268</v>
-      </c>
-      <c r="D26" t="s">
-        <v>121</v>
-      </c>
       <c r="E26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F26" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G26">
         <v>69.95</v>
@@ -2732,7 +2815,7 @@
         <v>49</v>
       </c>
       <c r="I26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M26">
         <v>130</v>
@@ -2741,7 +2824,7 @@
         <v>22</v>
       </c>
       <c r="U26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V26">
         <v>73</v>
@@ -2752,19 +2835,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" t="s">
+        <v>269</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" t="s">
         <v>123</v>
       </c>
-      <c r="C27" t="s">
-        <v>270</v>
-      </c>
-      <c r="D27" t="s">
-        <v>121</v>
-      </c>
-      <c r="E27" t="s">
-        <v>124</v>
-      </c>
       <c r="F27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G27">
         <v>149.94999999999999</v>
@@ -2773,7 +2856,7 @@
         <v>109</v>
       </c>
       <c r="I27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M27">
         <v>135</v>
@@ -2782,7 +2865,7 @@
         <v>24</v>
       </c>
       <c r="U27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V27">
         <v>76</v>
@@ -2793,16 +2876,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D28" t="s">
         <v>126</v>
       </c>
-      <c r="C28" t="s">
-        <v>260</v>
-      </c>
-      <c r="D28" t="s">
-        <v>127</v>
-      </c>
       <c r="E28" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="F28" t="s">
+        <v>381</v>
       </c>
       <c r="G28">
         <v>199.95</v>
@@ -2811,7 +2897,7 @@
         <v>139</v>
       </c>
       <c r="I28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N28">
         <v>116</v>
@@ -2820,7 +2906,7 @@
         <v>26</v>
       </c>
       <c r="U28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V28">
         <v>79</v>
@@ -2831,19 +2917,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F29" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G29">
         <v>99.95</v>
@@ -2852,7 +2938,7 @@
         <v>69</v>
       </c>
       <c r="I29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N29">
         <v>119</v>
@@ -2861,7 +2947,7 @@
         <v>28</v>
       </c>
       <c r="U29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V29">
         <v>82</v>
@@ -2872,19 +2958,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" t="s">
         <v>133</v>
       </c>
-      <c r="C30" t="s">
-        <v>271</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>134</v>
       </c>
-      <c r="E30" t="s">
-        <v>135</v>
-      </c>
       <c r="F30" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G30">
         <v>279.95</v>
@@ -2893,7 +2979,7 @@
         <v>189</v>
       </c>
       <c r="I30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N30">
         <v>122</v>
@@ -2902,7 +2988,7 @@
         <v>30</v>
       </c>
       <c r="U30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V30">
         <v>85</v>
@@ -2913,16 +2999,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" t="s">
+        <v>271</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" t="s">
         <v>138</v>
       </c>
-      <c r="C31" t="s">
-        <v>272</v>
-      </c>
-      <c r="D31" t="s">
-        <v>121</v>
-      </c>
-      <c r="E31" t="s">
-        <v>139</v>
+      <c r="F31" t="s">
+        <v>380</v>
       </c>
       <c r="G31">
         <v>94.95</v>
@@ -2931,7 +3020,7 @@
         <v>64</v>
       </c>
       <c r="I31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N31">
         <v>125</v>
@@ -2940,7 +3029,7 @@
         <v>32</v>
       </c>
       <c r="U31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V31">
         <v>88</v>
@@ -2951,25 +3040,25 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" t="s">
+        <v>140</v>
+      </c>
+      <c r="E32" t="s">
         <v>143</v>
       </c>
-      <c r="C32" t="s">
-        <v>142</v>
-      </c>
-      <c r="D32" t="s">
-        <v>141</v>
-      </c>
-      <c r="E32" t="s">
-        <v>144</v>
-      </c>
       <c r="F32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H32">
         <v>249</v>
       </c>
       <c r="J32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R32">
         <v>12</v>
@@ -2978,7 +3067,7 @@
         <v>13</v>
       </c>
       <c r="U32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V32">
         <v>91</v>
@@ -2989,19 +3078,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" t="s">
         <v>146</v>
       </c>
-      <c r="C33" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" t="s">
-        <v>116</v>
-      </c>
-      <c r="E33" t="s">
-        <v>147</v>
-      </c>
       <c r="F33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G33">
         <v>144.94999999999999</v>
@@ -3010,7 +3099,7 @@
         <v>99</v>
       </c>
       <c r="J33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -3022,7 +3111,7 @@
         <v>16</v>
       </c>
       <c r="U33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V33">
         <v>94</v>
@@ -3033,16 +3122,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" t="s">
-        <v>294</v>
+        <v>293</v>
+      </c>
+      <c r="F34" t="s">
+        <v>379</v>
       </c>
       <c r="G34">
         <v>99.95</v>
@@ -3057,7 +3149,7 @@
         <v>32</v>
       </c>
       <c r="U34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V34">
         <v>97</v>
@@ -3068,16 +3160,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" t="s">
+        <v>267</v>
+      </c>
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" t="s">
         <v>149</v>
-      </c>
-      <c r="C35" t="s">
-        <v>268</v>
-      </c>
-      <c r="D35" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" t="s">
-        <v>150</v>
       </c>
       <c r="G35">
         <v>69.95</v>
@@ -3086,7 +3178,7 @@
         <v>49</v>
       </c>
       <c r="I35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M35">
         <v>140</v>
@@ -3095,7 +3187,7 @@
         <v>35</v>
       </c>
       <c r="U35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V35">
         <v>100</v>
@@ -3106,19 +3198,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G36">
         <v>99.95</v>
@@ -3127,7 +3219,7 @@
         <v>69</v>
       </c>
       <c r="I36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N36">
         <v>130</v>
@@ -3136,7 +3228,7 @@
         <v>38</v>
       </c>
       <c r="U36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V36">
         <v>103</v>
@@ -3147,16 +3239,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C37" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E37" t="s">
-        <v>296</v>
+        <v>295</v>
+      </c>
+      <c r="F37" t="s">
+        <v>378</v>
       </c>
       <c r="G37">
         <v>119.95</v>
@@ -3171,7 +3266,7 @@
         <v>41</v>
       </c>
       <c r="U37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V37">
         <v>106</v>
@@ -3182,16 +3277,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E38" t="s">
-        <v>297</v>
+        <v>296</v>
+      </c>
+      <c r="F38" t="s">
+        <v>377</v>
       </c>
       <c r="G38">
         <v>119.95</v>
@@ -3206,7 +3304,7 @@
         <v>44</v>
       </c>
       <c r="U38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V38">
         <v>109</v>
@@ -3217,16 +3315,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" t="s">
+        <v>267</v>
+      </c>
+      <c r="D39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" t="s">
         <v>157</v>
       </c>
-      <c r="C39" t="s">
-        <v>268</v>
-      </c>
-      <c r="D39" t="s">
-        <v>155</v>
-      </c>
-      <c r="E39" t="s">
-        <v>158</v>
+      <c r="F39" t="s">
+        <v>376</v>
       </c>
       <c r="G39">
         <v>99.95</v>
@@ -3235,7 +3336,7 @@
         <v>59</v>
       </c>
       <c r="I39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M39">
         <v>146</v>
@@ -3244,7 +3345,7 @@
         <v>47</v>
       </c>
       <c r="U39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V39">
         <v>112</v>
@@ -3255,16 +3356,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>159</v>
+      </c>
+      <c r="C40" t="s">
+        <v>267</v>
+      </c>
+      <c r="D40" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" t="s">
         <v>160</v>
       </c>
-      <c r="C40" t="s">
-        <v>268</v>
-      </c>
-      <c r="D40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E40" t="s">
-        <v>161</v>
+      <c r="F40" t="s">
+        <v>375</v>
       </c>
       <c r="G40">
         <v>99.95</v>
@@ -3273,7 +3377,7 @@
         <v>59</v>
       </c>
       <c r="I40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M40">
         <v>150</v>
@@ -3282,7 +3386,7 @@
         <v>50</v>
       </c>
       <c r="U40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V40">
         <v>115</v>
@@ -3293,16 +3397,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
-        <v>298</v>
+        <v>297</v>
+      </c>
+      <c r="F41" t="s">
+        <v>374</v>
       </c>
       <c r="G41">
         <v>199.95</v>
@@ -3317,7 +3424,7 @@
         <v>53</v>
       </c>
       <c r="U41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V41">
         <v>118</v>
@@ -3328,16 +3435,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" t="s">
+        <v>259</v>
+      </c>
+      <c r="D42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" t="s">
         <v>164</v>
       </c>
-      <c r="C42" t="s">
-        <v>260</v>
-      </c>
-      <c r="D42" t="s">
-        <v>155</v>
-      </c>
-      <c r="E42" t="s">
-        <v>165</v>
+      <c r="F42" t="s">
+        <v>373</v>
       </c>
       <c r="G42">
         <v>279.95</v>
@@ -3346,7 +3456,7 @@
         <v>199</v>
       </c>
       <c r="I42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N42">
         <v>137</v>
@@ -3355,7 +3465,7 @@
         <v>56</v>
       </c>
       <c r="U42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V42">
         <v>121</v>
@@ -3366,28 +3476,28 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" t="s">
         <v>168</v>
       </c>
-      <c r="C43" t="s">
-        <v>167</v>
-      </c>
-      <c r="D43" t="s">
-        <v>155</v>
-      </c>
-      <c r="E43" t="s">
-        <v>169</v>
-      </c>
       <c r="F43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H43">
         <v>49.95</v>
       </c>
       <c r="I43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M43">
         <v>155</v>
@@ -3396,7 +3506,7 @@
         <v>18</v>
       </c>
       <c r="U43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V43">
         <v>124</v>
@@ -3407,28 +3517,28 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" t="s">
         <v>171</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" t="s">
         <v>172</v>
       </c>
-      <c r="D44" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" t="s">
-        <v>173</v>
-      </c>
       <c r="F44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H44">
         <v>29.95</v>
       </c>
       <c r="I44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M44">
         <v>157</v>
@@ -3440,7 +3550,7 @@
         <v>21</v>
       </c>
       <c r="U44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V44">
         <v>127</v>
@@ -3451,19 +3561,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C45" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E45" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F45" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G45">
         <v>129.94999999999999</v>
@@ -3478,7 +3588,7 @@
         <v>60</v>
       </c>
       <c r="U45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V45">
         <v>130</v>
@@ -3489,16 +3599,19 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E46" t="s">
-        <v>300</v>
+        <v>299</v>
+      </c>
+      <c r="F46" t="s">
+        <v>372</v>
       </c>
       <c r="G46">
         <v>129.94999999999999</v>
@@ -3513,7 +3626,7 @@
         <v>63</v>
       </c>
       <c r="U46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V46">
         <v>133</v>
@@ -3524,28 +3637,28 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H47">
         <v>399.95</v>
       </c>
       <c r="I47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M47">
         <v>163</v>
@@ -3554,7 +3667,7 @@
         <v>66</v>
       </c>
       <c r="U47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V47">
         <v>136</v>
@@ -3565,28 +3678,28 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H48">
         <v>159.94999999999999</v>
       </c>
       <c r="I48" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M48">
         <v>166</v>
@@ -3595,7 +3708,7 @@
         <v>69</v>
       </c>
       <c r="U48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V48">
         <v>139</v>
@@ -3606,28 +3719,28 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" t="s">
+        <v>266</v>
+      </c>
+      <c r="D49" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" t="s">
         <v>181</v>
       </c>
-      <c r="C49" t="s">
-        <v>267</v>
-      </c>
-      <c r="D49" t="s">
-        <v>70</v>
-      </c>
-      <c r="E49" t="s">
-        <v>182</v>
-      </c>
       <c r="F49" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H49">
         <v>149.94999999999999</v>
       </c>
       <c r="I49" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N49">
         <v>146</v>
@@ -3636,7 +3749,7 @@
         <v>72</v>
       </c>
       <c r="U49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V49">
         <v>142</v>
@@ -3647,28 +3760,28 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C50" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H50">
         <v>129.94999999999999</v>
       </c>
       <c r="I50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N50">
         <v>149</v>
@@ -3677,7 +3790,7 @@
         <v>75</v>
       </c>
       <c r="U50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V50">
         <v>145</v>
@@ -3688,28 +3801,28 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>188</v>
+      </c>
+      <c r="C51" t="s">
+        <v>187</v>
+      </c>
+      <c r="D51" t="s">
+        <v>69</v>
+      </c>
+      <c r="E51" t="s">
         <v>189</v>
       </c>
-      <c r="C51" t="s">
-        <v>188</v>
-      </c>
-      <c r="D51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E51" t="s">
-        <v>190</v>
-      </c>
       <c r="F51" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H51">
         <v>79.95</v>
       </c>
       <c r="I51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M51">
         <v>168</v>
@@ -3724,7 +3837,7 @@
         <v>25</v>
       </c>
       <c r="U51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V51">
         <v>148</v>
@@ -3735,16 +3848,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>192</v>
+      </c>
+      <c r="C52" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" t="s">
+        <v>191</v>
+      </c>
+      <c r="E52" t="s">
         <v>193</v>
       </c>
-      <c r="C52" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" t="s">
-        <v>192</v>
-      </c>
-      <c r="E52" t="s">
-        <v>194</v>
+      <c r="F52" t="s">
+        <v>371</v>
       </c>
       <c r="G52">
         <v>34.950000000000003</v>
@@ -3753,7 +3869,7 @@
         <v>25</v>
       </c>
       <c r="I52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K52">
         <v>1</v>
@@ -3765,7 +3881,7 @@
         <v>43</v>
       </c>
       <c r="U52" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V52">
         <v>151</v>
@@ -3776,16 +3892,19 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>195</v>
+      </c>
+      <c r="C53" t="s">
+        <v>281</v>
+      </c>
+      <c r="D53" t="s">
+        <v>191</v>
+      </c>
+      <c r="E53" t="s">
         <v>196</v>
       </c>
-      <c r="C53" t="s">
-        <v>282</v>
-      </c>
-      <c r="D53" t="s">
-        <v>192</v>
-      </c>
-      <c r="E53" t="s">
-        <v>197</v>
+      <c r="F53" t="s">
+        <v>370</v>
       </c>
       <c r="G53">
         <v>34.950000000000003</v>
@@ -3800,7 +3919,7 @@
         <v>46</v>
       </c>
       <c r="U53" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V53">
         <v>154</v>
@@ -3811,19 +3930,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>197</v>
+      </c>
+      <c r="C54" t="s">
+        <v>282</v>
+      </c>
+      <c r="D54" t="s">
         <v>198</v>
       </c>
-      <c r="C54" t="s">
-        <v>283</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>199</v>
       </c>
-      <c r="E54" t="s">
-        <v>200</v>
-      </c>
       <c r="F54" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G54">
         <v>49.95</v>
@@ -3832,7 +3951,7 @@
         <v>35</v>
       </c>
       <c r="I54" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O54">
         <v>1</v>
@@ -3841,7 +3960,7 @@
         <v>49</v>
       </c>
       <c r="U54" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V54">
         <v>157</v>
@@ -3852,16 +3971,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C55" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D55" t="s">
         <v>23</v>
       </c>
       <c r="E55" t="s">
-        <v>203</v>
+        <v>202</v>
+      </c>
+      <c r="F55" t="s">
+        <v>369</v>
       </c>
       <c r="G55">
         <v>49.95</v>
@@ -3870,7 +3992,7 @@
         <v>35</v>
       </c>
       <c r="I55" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K55">
         <v>1</v>
@@ -3882,7 +4004,7 @@
         <v>52</v>
       </c>
       <c r="U55" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V55">
         <v>160</v>
@@ -3893,19 +4015,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>204</v>
+      </c>
+      <c r="C56" t="s">
+        <v>284</v>
+      </c>
+      <c r="D56" t="s">
         <v>205</v>
       </c>
-      <c r="C56" t="s">
-        <v>285</v>
-      </c>
-      <c r="D56" t="s">
-        <v>206</v>
-      </c>
       <c r="E56" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F56" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G56">
         <v>24.95</v>
@@ -3923,7 +4045,7 @@
         <v>55</v>
       </c>
       <c r="U56" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V56">
         <v>163</v>
@@ -3934,19 +4056,19 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D57" t="s">
+        <v>206</v>
+      </c>
+      <c r="E57" t="s">
         <v>207</v>
       </c>
-      <c r="E57" t="s">
-        <v>208</v>
-      </c>
       <c r="F57" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G57">
         <v>39.950000000000003</v>
@@ -3955,7 +4077,7 @@
         <v>29</v>
       </c>
       <c r="I57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -3967,7 +4089,7 @@
         <v>58</v>
       </c>
       <c r="U57" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V57">
         <v>166</v>
@@ -3978,19 +4100,19 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>208</v>
+      </c>
+      <c r="C58" t="s">
+        <v>286</v>
+      </c>
+      <c r="D58" t="s">
+        <v>154</v>
+      </c>
+      <c r="E58" t="s">
         <v>209</v>
       </c>
-      <c r="C58" t="s">
-        <v>287</v>
-      </c>
-      <c r="D58" t="s">
-        <v>155</v>
-      </c>
-      <c r="E58" t="s">
-        <v>210</v>
-      </c>
       <c r="F58" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G58">
         <v>99.95</v>
@@ -3999,7 +4121,7 @@
         <v>69</v>
       </c>
       <c r="I58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O58">
         <v>1</v>
@@ -4011,7 +4133,7 @@
         <v>80</v>
       </c>
       <c r="U58" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V58">
         <v>169</v>
@@ -4022,28 +4144,28 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>211</v>
+      </c>
+      <c r="C59" t="s">
+        <v>289</v>
+      </c>
+      <c r="D59" t="s">
+        <v>154</v>
+      </c>
+      <c r="E59" t="s">
         <v>212</v>
       </c>
-      <c r="C59" t="s">
-        <v>290</v>
-      </c>
-      <c r="D59" t="s">
-        <v>155</v>
-      </c>
-      <c r="E59" t="s">
-        <v>213</v>
-      </c>
       <c r="F59" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H59">
         <v>29.95</v>
       </c>
       <c r="I59" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O59">
         <v>1</v>
@@ -4052,7 +4174,7 @@
         <v>27</v>
       </c>
       <c r="U59" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="V59">
         <v>172</v>
@@ -4063,25 +4185,25 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F60" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H60">
         <v>169</v>
       </c>
       <c r="J60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R60">
         <v>30</v>
@@ -4093,7 +4215,7 @@
         <v>20</v>
       </c>
       <c r="U60" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V60">
         <v>175</v>
@@ -4104,25 +4226,25 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>216</v>
+      </c>
+      <c r="C61" t="s">
+        <v>288</v>
+      </c>
+      <c r="D61" t="s">
         <v>217</v>
       </c>
-      <c r="C61" t="s">
-        <v>289</v>
-      </c>
-      <c r="D61" t="s">
-        <v>218</v>
-      </c>
       <c r="E61" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F61" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H61" s="1">
         <v>1299</v>
       </c>
       <c r="J61" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N61">
         <v>201</v>
@@ -4134,7 +4256,7 @@
         <v>3</v>
       </c>
       <c r="U61" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V61">
         <v>178</v>
@@ -4145,22 +4267,22 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>219</v>
+      </c>
+      <c r="C62" t="s">
+        <v>218</v>
+      </c>
+      <c r="D62" t="s">
         <v>220</v>
       </c>
-      <c r="C62" t="s">
-        <v>219</v>
-      </c>
-      <c r="D62" t="s">
-        <v>221</v>
-      </c>
       <c r="E62" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H62">
         <v>69.95</v>
       </c>
       <c r="J62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R62">
         <v>36</v>
@@ -4172,7 +4294,7 @@
         <v>23</v>
       </c>
       <c r="U62" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V62">
         <v>181</v>
@@ -4183,19 +4305,19 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>222</v>
+      </c>
+      <c r="C63" t="s">
+        <v>221</v>
+      </c>
+      <c r="D63" t="s">
         <v>223</v>
       </c>
-      <c r="C63" t="s">
-        <v>222</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>224</v>
       </c>
-      <c r="E63" t="s">
-        <v>225</v>
-      </c>
       <c r="F63" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G63">
         <v>74.95</v>
@@ -4204,13 +4326,13 @@
         <v>59</v>
       </c>
       <c r="I63" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="S63">
         <v>7</v>
       </c>
       <c r="U63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V63">
         <v>184</v>
@@ -4221,19 +4343,19 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C64" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E64" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G64">
         <v>149.94999999999999</v>
@@ -4242,7 +4364,7 @@
         <v>99</v>
       </c>
       <c r="I64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N64">
         <v>205</v>
@@ -4251,7 +4373,7 @@
         <v>9</v>
       </c>
       <c r="U64" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V64">
         <v>187</v>
@@ -4262,19 +4384,19 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C65" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D65" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E65" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F65" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G65">
         <v>149.94999999999999</v>
@@ -4289,7 +4411,7 @@
         <v>11</v>
       </c>
       <c r="U65" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V65">
         <v>190</v>
@@ -4300,25 +4422,25 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E66" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F66" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H66">
         <v>74.95</v>
       </c>
       <c r="J66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M66">
         <v>172</v>
@@ -4330,7 +4452,7 @@
         <v>13</v>
       </c>
       <c r="U66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V66">
         <v>193</v>
@@ -4341,22 +4463,22 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C67" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D67" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E67" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H67">
         <v>24.95</v>
       </c>
       <c r="J67" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N67">
         <v>30</v>
@@ -4376,22 +4498,22 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>237</v>
+      </c>
+      <c r="C68" t="s">
+        <v>236</v>
+      </c>
+      <c r="D68" t="s">
         <v>238</v>
       </c>
-      <c r="C68" t="s">
-        <v>237</v>
-      </c>
-      <c r="D68" t="s">
-        <v>239</v>
-      </c>
       <c r="E68" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H68">
         <v>29.95</v>
       </c>
       <c r="I68" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N68">
         <v>33</v>
@@ -4411,13 +4533,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>239</v>
+      </c>
+      <c r="D69" t="s">
         <v>240</v>
       </c>
-      <c r="D69" t="s">
-        <v>241</v>
-      </c>
       <c r="E69" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H69">
         <v>19.95</v>
@@ -4440,13 +4562,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D70" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E70" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H70">
         <v>24.95</v>
@@ -4469,13 +4591,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E71" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H71">
         <v>24.95</v>
@@ -4498,13 +4620,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D72" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E72" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H72">
         <v>24.95</v>
@@ -4527,13 +4649,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E73" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H73">
         <v>19.95</v>
@@ -4556,13 +4678,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D74" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E74" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H74">
         <v>29.95</v>
@@ -4585,13 +4707,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E75" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H75">
         <v>24.95</v>
@@ -4614,19 +4736,19 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C76" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E76" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F76" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H76">
         <v>449</v>
@@ -4649,13 +4771,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D77" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E77" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H77">
         <v>19.95</v>
@@ -4678,13 +4800,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D78" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E78" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H78">
         <v>19.95</v>
@@ -4707,25 +4829,25 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>251</v>
+      </c>
+      <c r="C79" t="s">
+        <v>253</v>
+      </c>
+      <c r="D79" t="s">
         <v>252</v>
       </c>
-      <c r="C79" t="s">
-        <v>254</v>
-      </c>
-      <c r="D79" t="s">
-        <v>253</v>
-      </c>
       <c r="E79" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F79" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H79">
         <v>59.95</v>
       </c>
       <c r="J79" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T79">
         <v>62</v>
@@ -4742,16 +4864,16 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C80" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D80" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E80" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H80">
         <v>199.95</v>

</xml_diff>